<commit_message>
Change the Transversal Themes data input sheet
Match the identifiers in the Mapping sheet in the values sheet.
Normalize codes. Include mapping sheet in the worksheet.
</commit_message>
<xml_diff>
--- a/data/rtei_data_2015.xlsx
+++ b/data/rtei_data_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="812" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="551" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Core Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,16 +17,17 @@
     <sheet name="Zimbabwe Summary" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Country Comparison" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Transversal Themes" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Transversal Themes Mappings" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3805" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1378">
   <si>
     <t>Theme</t>
   </si>
@@ -3709,118 +3710,457 @@
     <t>Transversal Themes</t>
   </si>
   <si>
-    <t>1. Opportunity and Indirect Costs</t>
-  </si>
-  <si>
-    <t>2. National Normative Framework</t>
-  </si>
-  <si>
-    <t>3. Monitoring and Accountability</t>
-  </si>
-  <si>
-    <t>4. Content of Education</t>
-  </si>
-  <si>
-    <t>5. Income Inequality</t>
-  </si>
-  <si>
-    <t>6. Teachers</t>
-  </si>
-  <si>
-    <t>7. Private Education</t>
-  </si>
-  <si>
-    <t>8. Girls' Education</t>
-  </si>
-  <si>
-    <t>9. Indigenous and Minority Populations</t>
-  </si>
-  <si>
-    <t>10. Children with Disabilities</t>
-  </si>
-  <si>
-    <t>11. Regional Disparities</t>
-  </si>
-  <si>
-    <t>12. Alignment of Education Aims</t>
-  </si>
-  <si>
-    <t>1A. Legal restrictions in opportunity and indirect costs</t>
-  </si>
-  <si>
-    <t>1B. Opportunity and indirect costs in practice</t>
-  </si>
-  <si>
-    <t>2A. National Normative Framework</t>
-  </si>
-  <si>
-    <t>3A. Strength of monitoring and accountability</t>
-  </si>
-  <si>
-    <t>4A. Availability of textbooks</t>
-  </si>
-  <si>
-    <t>4B. Content of curriculum</t>
-  </si>
-  <si>
-    <t>5A. Relative enrollment and completion rates</t>
-  </si>
-  <si>
-    <t>5B. Achievement across income quintiles</t>
-  </si>
-  <si>
-    <t>6A. Effect of Teacher Training</t>
-  </si>
-  <si>
-    <t>6B. Content of teacher training</t>
-  </si>
-  <si>
-    <t>7A. Private education legal environment</t>
-  </si>
-  <si>
-    <t>7B.A Relative teacher salary</t>
-  </si>
-  <si>
-    <t>7B.B Relative gross enrollment patterns</t>
-  </si>
-  <si>
-    <t>8A. Overall state of girls' education</t>
-  </si>
-  <si>
-    <t>8B. Discriminatory environment</t>
-  </si>
-  <si>
-    <t>8C. Relative state of girls' education</t>
-  </si>
-  <si>
-    <t>9A. Discriminatory environment</t>
-  </si>
-  <si>
-    <t>10A.A Structure and support</t>
-  </si>
-  <si>
-    <t>10A.B Participation and achievement</t>
-  </si>
-  <si>
-    <t>10A.C Overall state of education for children with disabilities</t>
-  </si>
-  <si>
-    <t>11A. Relative state of children in rural settings</t>
-  </si>
-  <si>
-    <t>12A. Alignment of education aims</t>
+    <t>1: Children with Disabilities</t>
+  </si>
+  <si>
+    <t>2: Content of Education</t>
+  </si>
+  <si>
+    <t>3: Girls' Education</t>
+  </si>
+  <si>
+    <t>4: Indigenous and Minority Populations</t>
+  </si>
+  <si>
+    <t>5: Monitoring and Accountability</t>
+  </si>
+  <si>
+    <t>6: National Normative Framework</t>
+  </si>
+  <si>
+    <t>7: Opportunity and Indirect Costs</t>
+  </si>
+  <si>
+    <t>8: Private Education</t>
+  </si>
+  <si>
+    <t>9: Teachers</t>
+  </si>
+  <si>
+    <t>10: Income Inequality</t>
+  </si>
+  <si>
+    <t>11: Regional Disparities</t>
+  </si>
+  <si>
+    <t>12: Alignment of Education Aims</t>
+  </si>
+  <si>
+    <t>1A.A: Structure and support</t>
+  </si>
+  <si>
+    <t>1A.B: Participation and achievement</t>
+  </si>
+  <si>
+    <t>1A.C: Overall state of education for children with disabilities</t>
+  </si>
+  <si>
+    <t>2A: Content of curriculum</t>
+  </si>
+  <si>
+    <t>2B: Availability of textbooks</t>
+  </si>
+  <si>
+    <t>3A: Overall state of girls' education</t>
+  </si>
+  <si>
+    <t>3B: Discriminatory environment</t>
+  </si>
+  <si>
+    <t>3C: Relative state of girls' education</t>
+  </si>
+  <si>
+    <t>4A: Discriminatory environment</t>
+  </si>
+  <si>
+    <t>5A: Strength of monitoring and accountability</t>
+  </si>
+  <si>
+    <t>6A: National Normative Framework</t>
+  </si>
+  <si>
+    <t>7A: Legal restrictions in opportunity and indirect costs</t>
+  </si>
+  <si>
+    <t>7B: Opportunity and indirect costs in practice</t>
+  </si>
+  <si>
+    <t>8A: Private education legal environment</t>
+  </si>
+  <si>
+    <t>8B.A: Relative teacher salary</t>
+  </si>
+  <si>
+    <t>8B.B: Relative gross enrollment patterns</t>
+  </si>
+  <si>
+    <t>9A: Content of teacher training</t>
+  </si>
+  <si>
+    <t>9B: Effect of Teacher Training</t>
+  </si>
+  <si>
+    <t>10A: Relative enrollment and completion rates</t>
+  </si>
+  <si>
+    <t>10B: Achievement across income quintiles</t>
+  </si>
+  <si>
+    <t>11A: Relative state of children in rural settings</t>
+  </si>
+  <si>
+    <t>12A: Alignment of education aims</t>
+  </si>
+  <si>
+    <t>Data Unavailable</t>
   </si>
   <si>
     <t>See analytic handbook for interpretation</t>
   </si>
   <si>
-    <t>Data Unavailable</t>
-  </si>
-  <si>
     <t>See analytic handbook for visual</t>
   </si>
   <si>
     <t>See chart below</t>
+  </si>
+  <si>
+    <t>Level 1: Category</t>
+  </si>
+  <si>
+    <t>1. Children with Disabilities</t>
+  </si>
+  <si>
+    <t>2. Content of Education</t>
+  </si>
+  <si>
+    <t>3. Girls' Education</t>
+  </si>
+  <si>
+    <t>4. Indigenous and Minority Populations</t>
+  </si>
+  <si>
+    <t>5. Monitoring and Accountability</t>
+  </si>
+  <si>
+    <t>6. National Normative Framework</t>
+  </si>
+  <si>
+    <t>7. Opportunity and Indirect Costs</t>
+  </si>
+  <si>
+    <t>8. Private Education</t>
+  </si>
+  <si>
+    <t>9. Teachers</t>
+  </si>
+  <si>
+    <t>Level 2: Transversal Theme</t>
+  </si>
+  <si>
+    <t>1A. Structure and support </t>
+  </si>
+  <si>
+    <t>2A. Content of curriculum</t>
+  </si>
+  <si>
+    <t>3A. Overall state of girls' education</t>
+  </si>
+  <si>
+    <t>3B. Discriminatory environment</t>
+  </si>
+  <si>
+    <t>4A. Discriminatory environment</t>
+  </si>
+  <si>
+    <t>5A. Strength of monitoring and accountability</t>
+  </si>
+  <si>
+    <t>6A. National Normative Framework</t>
+  </si>
+  <si>
+    <t>7A. Legal restrictions in opportunity and indirect costs</t>
+  </si>
+  <si>
+    <t>7B. Opportunity and indirect costs in practice</t>
+  </si>
+  <si>
+    <t>8A. Private education legal environment</t>
+  </si>
+  <si>
+    <t>9A. Content of teacher training</t>
+  </si>
+  <si>
+    <t>Level 3: Indicators</t>
+  </si>
+  <si>
+    <t>1.4.4j: Is data disaggregated by disability status?</t>
+  </si>
+  <si>
+    <t>4.1.2a: Does the national curriculum direct education towards the full development of the child’s personality, talents, and mental and physical abilities?</t>
+  </si>
+  <si>
+    <t>1.4.4b: Is data disaggregated by sex?</t>
+  </si>
+  <si>
+    <t>1.2.4: Do national laws protect the rights of minorities to establish private schools?</t>
+  </si>
+  <si>
+    <t>1.2.1a: Do national laws protect the right to primary education? </t>
+  </si>
+  <si>
+    <t>3.1.4a - Are tuition fees charged for public university/higher education in 2014?</t>
+  </si>
+  <si>
+    <t>4.1.3a: Does the required training for teachers include improving the skills necessary for teaching towards the full development of the child’s personality, talents, and mental and physical abilities?</t>
+  </si>
+  <si>
+    <t>3.2.1j: Do national laws forbid discrimination in education by disability status?</t>
+  </si>
+  <si>
+    <t>4.1.2b: Does the national curriculum direct education towards the full development of respect for human rights and fundamental freedoms?</t>
+  </si>
+  <si>
+    <t>3.2.1b: Do national laws forbid discrimination in education by sex?</t>
+  </si>
+  <si>
+    <t>5.4.1a: Does national law prohibit early marriage (below the age of 18)?</t>
+  </si>
+  <si>
+    <t>3.1.2 - What percent of household spending was spent on primary education in 2013?</t>
+  </si>
+  <si>
+    <t>4.1.3b: Does the required training for teachers include improving the skills necessary for teaching towards the full development of respect for human rights and fundamental freedoms?</t>
+  </si>
+  <si>
+    <t>5.1.1: Do national laws recognize the right to education for children with disabilities</t>
+  </si>
+  <si>
+    <t>4.1.2c: Does the national curriculum direct education towards the full development of respect for the child’s parents, cultural identity, language, and values, as well as respect for the values of the child’s country and other civilizations?</t>
+  </si>
+  <si>
+    <t>3.2.2a: Is the expulsion of girls from school because of pregnancy or for having a baby explicitly forbidden in legislation?</t>
+  </si>
+  <si>
+    <t>5.2.1a: Do national laws prohibit early marriage (before the age of 18)?</t>
+  </si>
+  <si>
+    <t>1.4.4a: Is data disaggregated by race and color (ethnicity)?</t>
+  </si>
+  <si>
+    <t>1.2.1c: Do national laws protect the right to technical and vocational training?</t>
+  </si>
+  <si>
+    <t>5.4.2: Is the legal minimum age of employment 15 or above?</t>
+  </si>
+  <si>
+    <t>3.1.3 - What percent of household spending was spent on secondary education in 2013?</t>
+  </si>
+  <si>
+    <t>4.1.3c: Does the required training for teachers include improving the skills necessary for teaching towards the full development of respect for the child’s parents, cultural identity, language, and values, as well as respect for the values of the child’s country and other civilizations?</t>
+  </si>
+  <si>
+    <t>5.1.2: Are reasonable accommodation measures available for children with disabilities in mainstream schools?</t>
+  </si>
+  <si>
+    <t>Q 4.1.2d: Does the national curriculum direct education towards the full development of the child’s responsibilities in a free society, including understanding peace, tolerance, equality, and friendship among all persons and groups?</t>
+  </si>
+  <si>
+    <t>1.4.4c: Is data disaggregated by language?</t>
+  </si>
+  <si>
+    <t>4.2.1: Has the national government adopted specific measures to protect children from violence and abuse in school?</t>
+  </si>
+  <si>
+    <t>5.4.5a: Is the legal minimum age of military recruitment 15 or above?</t>
+  </si>
+  <si>
+    <t>5.4.1b: What percent of women were married by the age of 18?</t>
+  </si>
+  <si>
+    <t>4.1.3d: Does the required training for teachers include improving the skills necessary for teaching towards the full development of the child’s responsibilities in a free society, including understanding peace, tolerance, equality, and friendship among all persons and groups?</t>
+  </si>
+  <si>
+    <t>5.1.3: What is the percentage of teachers trained to teach children with disabilities?</t>
+  </si>
+  <si>
+    <t>4.1.2e: Does the national curriculum direct education towards the full development of respect for the natural environment?</t>
+  </si>
+  <si>
+    <t>3.3.1ac: What is the gross primary school enrollment rate for females?</t>
+  </si>
+  <si>
+    <t>1.4.4d: Is data disaggregated by religion?</t>
+  </si>
+  <si>
+    <t>5.4.3: Has the government adopted specific measures to combat child labor?</t>
+  </si>
+  <si>
+    <t>5.4.4: What percent of children under the age of 15 worked in the labor force?</t>
+  </si>
+  <si>
+    <t>4.1.3e: Does the required training for teachers include improving the skills necessary for teaching towards the full development of respect for the natural environment?</t>
+  </si>
+  <si>
+    <t>4.1.5a: Does the national curriculum include health and well-being?</t>
+  </si>
+  <si>
+    <t>3.3.2ac: What is the net primary school enrollment rate for females?</t>
+  </si>
+  <si>
+    <t>1.4.4f: Is data disaggregated by national or social origin?</t>
+  </si>
+  <si>
+    <t>1.4.3: How often is data on education regularly collected and made publicly available?</t>
+  </si>
+  <si>
+    <t>5.4.5b: Are children under the age of 15 recruited by the military in practice?</t>
+  </si>
+  <si>
+    <t>4.1.5b: Does the national curriculum include human rights?</t>
+  </si>
+  <si>
+    <t>3.3.4ac: What is the public primary school completion rate for females?</t>
+  </si>
+  <si>
+    <t>1.4.4i: Is data disaggregated by sexual orientation and gender identity?</t>
+  </si>
+  <si>
+    <t>4.1.5c: Does the national curriculum include the arts?</t>
+  </si>
+  <si>
+    <t>3.3.4ec: What is the private primary school completion rate for females?</t>
+  </si>
+  <si>
+    <t>1.4.4l: Is data disaggregated by nationality?</t>
+  </si>
+  <si>
+    <t>3.2.1a: Do national laws forbid discrimination in education by race and color (ethnicity)?</t>
+  </si>
+  <si>
+    <t>1.3.1b: Are there targeted implementation dates for each stage in the progressive realization of the plan?</t>
+  </si>
+  <si>
+    <t>3.2.1c: Do national laws forbid discrimination in education by language?</t>
+  </si>
+  <si>
+    <t>4.3.1ac: What percent of females received an overall passing score on the national assessment/exam?</t>
+  </si>
+  <si>
+    <t>3.2.1d: Do national laws forbid discrimination in education by religion?</t>
+  </si>
+  <si>
+    <t>4.3.1bc: What percent of females received a passing score on the national reading assessment/exam?</t>
+  </si>
+  <si>
+    <t>3.2.1f: Do national laws forbid discrimination in education by national or social origin?</t>
+  </si>
+  <si>
+    <t>3.1.1: Do national laws provide for free and compulsory education?</t>
+  </si>
+  <si>
+    <t>4.3.1cc: What percent of females received a passing score on the national mathematics assessment/exam?</t>
+  </si>
+  <si>
+    <t>3.2.1i: Do national laws forbid discrimination in education by sexual orientation and gender identity?</t>
+  </si>
+  <si>
+    <t>3.2.1a: Do national laws forbid discrimination in education on race and color (ethnicity)?</t>
+  </si>
+  <si>
+    <t>4.3.2ac: What if the youth literacy rate (ages 15-24) for females?</t>
+  </si>
+  <si>
+    <t>3.2.1l: Do national laws forbid discrimination in education by nationality?</t>
+  </si>
+  <si>
+    <t>3.2.1b: Do national laws forbid discrimination in education on sex?</t>
+  </si>
+  <si>
+    <t>4.3.2bc: What is the adult literacy rate (age 15+) for females?</t>
+  </si>
+  <si>
+    <t>3.2.1c: Do national laws forbid discrimination in education on language?</t>
+  </si>
+  <si>
+    <t>5.2.1: Are there mobile schools for children of nomads</t>
+  </si>
+  <si>
+    <t>3.2.1d: Do national laws forbid discrimination in education on religion?</t>
+  </si>
+  <si>
+    <t>5.2.2: Do national laws provide for language of instruction to be in the child’s mother tongue?</t>
+  </si>
+  <si>
+    <t>3.2.1e: Do national laws forbid discrimination in education on political and other opinion?</t>
+  </si>
+  <si>
+    <t>5.2.3a: What percentage of students are not taught in their mother tongue?</t>
+  </si>
+  <si>
+    <t>3.2.1f: Do national laws forbid discrimination in education on national or social orgin?</t>
+  </si>
+  <si>
+    <t>3.2.1g: Do national laws forbid discrimination in education on property?</t>
+  </si>
+  <si>
+    <t>3.2.1h: Do national laws forbid discrimination in education on birth?</t>
+  </si>
+  <si>
+    <t>3.2.1i: Do national laws forbid discrimination in education on sexual orientation and gender identity?</t>
+  </si>
+  <si>
+    <t>3.2.1j: Do national laws forbid discrimination in education on disability?</t>
+  </si>
+  <si>
+    <t>3.2.1k: Do national laws forbid discrimination in education on age?</t>
+  </si>
+  <si>
+    <t>3.2.1l: Do national laws forbid discrimination in education on nationality?</t>
+  </si>
+  <si>
+    <t>3.2.1m: Do national laws forbid discrimination in education on marital and family status?</t>
+  </si>
+  <si>
+    <t>3.2.1n: Do national laws forbid discrimination in education on health status?</t>
+  </si>
+  <si>
+    <t>3.2.1o: Do national laws forbid discrimination in education on place of residence?</t>
+  </si>
+  <si>
+    <t>3.2.1p: Do national laws forbid discrimination in education on economic and social situation?</t>
+  </si>
+  <si>
+    <t>4.1.1a: Do national laws or policies direct education towards the full development of the child’s personality, talents, and mental and physical abilities?</t>
+  </si>
+  <si>
+    <t>4.1.1b: Do national laws or policies direct education towards the full development of respect for human rights and fundamental freedoms?</t>
+  </si>
+  <si>
+    <t>4.1.1c: Do national laws or policies direct education towards the full development of respect for the child’s parents, cultural identity, language, and values, as well as respect for the values of the child’s country and other civilizations?</t>
+  </si>
+  <si>
+    <t>4.1.1d: Do national laws or policies direct education towards the full development of the child’s responsibilities in a free society, including understanding peace, tolerance, equality, and friendship among all persons and groups?</t>
+  </si>
+  <si>
+    <t>4.1.1e: Do national laws or policies direct education towards the full development of respect for the natural environment?</t>
+  </si>
+  <si>
+    <t>4.1.4: Are there established mechanisms to ensure that textbooks used in both the public and private schools are aligned with the curriculum guidelines provided by the Ministry of Education?</t>
+  </si>
+  <si>
+    <t>5.1.1: Do national laws recognize the right to education for children with minorities?</t>
+  </si>
+  <si>
+    <t>1.3.2: Does the national education plan include measures to encourage regular attendance and reduce drop-out rates?</t>
+  </si>
+  <si>
+    <t>3.1.5: Is basic education publicly provided for adults who have not completed primary education?</t>
+  </si>
+  <si>
+    <t>4.1.6: Do national laws include children in the decision making process of school curricula, school policies, and codes of behavior?</t>
+  </si>
+  <si>
+    <t>5.4.1a: Do national laws prohibit early marriage (before the age of 18)?</t>
   </si>
 </sst>
 </file>
@@ -3833,7 +4173,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3872,12 +4212,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4056,7 +4390,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4212,7 +4546,817 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4f81bd"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$B$21:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c0504d"/>
+            </a:solidFill>
+            <a:ln w="25560">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$E$21:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="22352211"/>
+        <c:axId val="86315210"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="22352211"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>School Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="86315210"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86315210"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Gross Enrollment Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="22352211"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4f81bd"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$B$22:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c0504d"/>
+            </a:solidFill>
+            <a:ln w="25560">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$E$22:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="34804857"/>
+        <c:axId val="22661935"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="34804857"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>School Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="22661935"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="22661935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Gross Enrollment Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="34804857"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4f81bd"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$B$23:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c0504d"/>
+            </a:solidFill>
+            <a:ln w="25560">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$E$23:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="27788400"/>
+        <c:axId val="46336699"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="27788400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>School Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="46336699"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="46336699"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Gross Enrollment Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="27788400"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4352,11 +5496,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="44168113"/>
-        <c:axId val="36640075"/>
+        <c:axId val="57373275"/>
+        <c:axId val="19104153"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="44168113"/>
+        <c:axId val="57373275"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4396,14 +5540,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="36640075"/>
+        <c:crossAx val="19104153"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36640075"/>
+        <c:axId val="19104153"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4450,817 +5594,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44168113"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4f81bd"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$B$21:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0504d"/>
-            </a:solidFill>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$E$21:$G$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="22990638"/>
-        <c:axId val="84326149"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="22990638"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>School Level</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="84326149"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="84326149"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Gross Enrollment Rate</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="22990638"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4f81bd"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$B$22:$D$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0504d"/>
-            </a:solidFill>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$E$22:$G$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="62023056"/>
-        <c:axId val="44680561"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="62023056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>School Level</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="44680561"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="44680561"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Gross Enrollment Rate</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="62023056"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4f81bd"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$29</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$B$23:$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0504d"/>
-            </a:solidFill>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$29</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$E$23:$F$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="43445498"/>
-        <c:axId val="1845583"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="43445498"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>School Level</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="1845583"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1845583"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Gross Enrollment Rate</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="43445498"/>
+        <c:crossAx val="57373275"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5300,16 +5634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1280880</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>796320</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>320760</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5317,8 +5651,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="22177080" y="4744440"/>
-        <a:ext cx="5847840" cy="2742480"/>
+        <a:off x="20000520" y="4269240"/>
+        <a:ext cx="5847120" cy="2513520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5330,16 +5664,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1063800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>598320</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>529560</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>63720</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>82080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5347,8 +5681,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28292400" y="4753800"/>
-        <a:ext cx="6273000" cy="2742480"/>
+        <a:off x="26125200" y="4278600"/>
+        <a:ext cx="6272640" cy="2513520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5360,16 +5694,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1280880</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>796320</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>320760</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5377,8 +5711,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="22177080" y="7601760"/>
-        <a:ext cx="5847840" cy="2742840"/>
+        <a:off x="20000520" y="6898320"/>
+        <a:ext cx="5847120" cy="2513880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5390,16 +5724,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1082880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>607680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>73080</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5407,8 +5741,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28311480" y="7601760"/>
-        <a:ext cx="6273000" cy="2742840"/>
+        <a:off x="26134560" y="6898320"/>
+        <a:ext cx="6272640" cy="2513880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5451,7 +5785,7 @@
   </sheetPr>
   <dimension ref="A1:AMF11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="AKY1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="ALB11" activeCellId="0" sqref="ALB11"/>
@@ -5658,6 +5992,7 @@
     <col collapsed="false" hidden="false" max="312" min="312" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="313" min="313" style="0" width="17.4251012145749"/>
     <col collapsed="false" hidden="false" max="314" min="314" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="315" min="315" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="317" min="316" style="0" width="23.2793522267206"/>
     <col collapsed="false" hidden="false" max="319" min="318" style="0" width="22.5748987854251"/>
     <col collapsed="false" hidden="false" max="321" min="320" style="0" width="24.1457489878543"/>
@@ -5785,6 +6120,7 @@
     <col collapsed="false" hidden="false" max="511" min="511" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="512" min="512" style="0" width="17.4251012145749"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="516" min="515" style="0" width="29.2874493927125"/>
     <col collapsed="false" hidden="false" max="518" min="517" style="0" width="28.5708502024291"/>
     <col collapsed="false" hidden="false" max="520" min="519" style="0" width="30.2874493927125"/>
@@ -5839,8 +6175,10 @@
     <col collapsed="false" hidden="false" max="601" min="601" style="0" width="9"/>
     <col collapsed="false" hidden="false" max="602" min="602" style="0" width="12.1417004048583"/>
     <col collapsed="false" hidden="false" max="603" min="603" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="604" min="604" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="605" min="605" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="606" min="606" style="0" width="17.8542510121458"/>
+    <col collapsed="false" hidden="false" max="607" min="607" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="608" min="608" style="0" width="17.2834008097166"/>
     <col collapsed="false" hidden="false" max="609" min="609" style="0" width="10.5708502024292"/>
     <col collapsed="false" hidden="false" max="610" min="610" style="0" width="13.8542510121457"/>
@@ -5977,6 +6315,7 @@
     <col collapsed="false" hidden="false" max="821" min="821" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="822" min="822" style="0" width="17.4251012145749"/>
     <col collapsed="false" hidden="false" max="823" min="823" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="824" min="824" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="826" min="825" style="0" width="32.5708502024291"/>
     <col collapsed="false" hidden="false" max="828" min="827" style="0" width="31.8582995951417"/>
     <col collapsed="false" hidden="false" max="830" min="829" style="0" width="33.4291497975709"/>
@@ -6030,8 +6369,10 @@
     <col collapsed="false" hidden="false" max="911" min="911" style="0" width="9"/>
     <col collapsed="false" hidden="false" max="912" min="912" style="0" width="12.1417004048583"/>
     <col collapsed="false" hidden="false" max="913" min="913" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="914" min="914" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="915" min="915" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="916" min="916" style="0" width="17.8542510121458"/>
+    <col collapsed="false" hidden="false" max="917" min="917" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="918" min="918" style="0" width="17.2834008097166"/>
     <col collapsed="false" hidden="false" max="919" min="919" style="0" width="10.5708502024292"/>
     <col collapsed="false" hidden="false" max="920" min="920" style="0" width="13.8542510121457"/>
@@ -20006,6 +20347,609 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AF50"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.4291497975708"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2348178137652"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.7125506072874"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="215.421052631579"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.4291497975708"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="109.854251012146"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.7165991902834"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="109.854251012146"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.1417004048583"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.4291497975708"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="153.570850202429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="33.8582995951417"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="42.1417004048583"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="171.425101214575"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="80.1376518218624"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="32.8582995951417"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="212.279352226721"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="30.7125506072874"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="49.5668016194332"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="66.5708502024292"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="41.4251012145749"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="80.1376518218624"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="28.5708502024291"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="37.4291497975708"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="153.570850202429"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="30.1417004048583"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="28.5708502024291"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="253.858299595142"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>1269</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>1273</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>1277</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>1280</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>1282</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>1283</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>1285</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>1293</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="0" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>1298</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>1299</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="0" t="s">
+        <v>1301</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>1302</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>1303</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>1305</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>1306</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>1308</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="0" t="s">
+        <v>1310</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>1311</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>1303</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>1312</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>1313</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>1315</v>
+      </c>
+      <c r="AF6" s="0" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>1318</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>1319</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>1315</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>1320</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>1321</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>1322</v>
+      </c>
+      <c r="AF7" s="0" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="0" t="s">
+        <v>1324</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>1325</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>1327</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="s">
+        <v>1329</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>1330</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>1331</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>1310</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="s">
+        <v>1332</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>1334</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="0" t="s">
+        <v>1315</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>1335</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>1337</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="0" t="s">
+        <v>1338</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>1339</v>
+      </c>
+      <c r="U13" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="0" t="s">
+        <v>1340</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>1341</v>
+      </c>
+      <c r="U14" s="0" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="0" t="s">
+        <v>1343</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>1344</v>
+      </c>
+      <c r="U15" s="0" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="0" t="s">
+        <v>1346</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>1347</v>
+      </c>
+      <c r="U16" s="0" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="0" t="s">
+        <v>1349</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="U17" s="0" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O18" s="0" t="s">
+        <v>1351</v>
+      </c>
+      <c r="U18" s="0" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O19" s="0" t="s">
+        <v>1353</v>
+      </c>
+      <c r="U19" s="0" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O20" s="0" t="s">
+        <v>1355</v>
+      </c>
+      <c r="U20" s="0" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U21" s="0" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U22" s="0" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U23" s="0" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U24" s="0" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U25" s="0" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U26" s="0" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U27" s="0" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U28" s="0" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U29" s="0" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U30" s="0" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U31" s="0" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U32" s="0" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U33" s="0" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U34" s="0" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U35" s="0" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U36" s="0" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U37" s="0" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U38" s="0" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U39" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U40" s="0" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U41" s="0" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U42" s="0" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U43" s="0" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U44" s="0" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U45" s="0" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U46" s="0" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U47" s="0" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U48" s="0" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U49" s="0" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U50" s="0" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -22797,7 +23741,7 @@
       </c>
       <c r="B14" s="13" t="n">
         <f aca="false">AVERAGE(B15:B17)</f>
-        <v>94.2333333333333</v>
+        <v>94.2333333333334</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23919,7 +24863,7 @@
       </c>
       <c r="J14" s="13" t="n">
         <f aca="false">'Philippines Summary'!B14</f>
-        <v>94.2333333333333</v>
+        <v>94.2333333333334</v>
       </c>
       <c r="K14" s="13" t="n">
         <f aca="false">'Tanzania Summary'!B14</f>
@@ -23971,7 +24915,7 @@
       </c>
       <c r="B16" s="27" t="n">
         <f aca="false">J14</f>
-        <v>94.2333333333333</v>
+        <v>94.2333333333334</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="21" t="s">
@@ -24388,27 +25332,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X16" activeCellId="0" sqref="X16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="34" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="34" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="19.1376518218624"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="34" t="s">
         <v>1226</v>
       </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
@@ -24425,35 +25364,46 @@
       <c r="U1" s="0"/>
       <c r="V1" s="0"/>
       <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="34" t="s">
         <v>1227</v>
       </c>
       <c r="C2" s="0"/>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="0"/>
+      <c r="E2" s="34" t="s">
         <v>1228</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="G2" s="34" t="s">
         <v>1229</v>
       </c>
-      <c r="F2" s="34" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G2" s="0"/>
-      <c r="H2" s="34" t="s">
-        <v>1231</v>
-      </c>
+      <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="34" t="s">
+        <v>1230</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>1231</v>
+      </c>
+      <c r="L2" s="34" t="s">
         <v>1232</v>
       </c>
-      <c r="K2" s="0"/>
-      <c r="L2" s="34" t="s">
+      <c r="M2" s="34" t="s">
         <v>1233</v>
       </c>
-      <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="O2" s="34" t="s">
         <v>1234</v>
@@ -24463,10 +25413,9 @@
       <c r="R2" s="34" t="s">
         <v>1235</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="T2" s="34" t="s">
         <v>1236</v>
       </c>
-      <c r="T2" s="0"/>
       <c r="U2" s="0"/>
       <c r="V2" s="34" t="s">
         <v>1237</v>
@@ -24474,8 +25423,19 @@
       <c r="W2" s="34" t="s">
         <v>1238</v>
       </c>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="34" t="s">
         <v>1239</v>
@@ -24543,408 +25503,467 @@
       <c r="W3" s="34" t="s">
         <v>1260</v>
       </c>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="34" t="s">
         <v>1051</v>
       </c>
-      <c r="B4" s="35" t="n">
+      <c r="B4" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DQ$5,'Core Questionnaire'!$GN$5,'Core Questionnaire'!$ALD$5,'Core Questionnaire'!$ALF$5,'Companion Questionnaire'!$BX$5)*100</f>
+        <v>68.4</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E4" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZM$5:$ZU$5,'Core Questionnaire'!$AAI$5:$AAM$5)*100</f>
+        <v>100</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="G4" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$5,'Core Questionnaire'!$FX$5,'Core Questionnaire'!$HC$5,'Companion Questionnaire'!$CE$5,'Core Questionnaire'!$HP$5,'Core Questionnaire'!$MP$5,'Core Questionnaire'!$PG$5,'Core Questionnaire'!$UE$5,'Companion Questionnaire'!$CG$5,'Core Questionnaire'!$HE$5,'Core Questionnaire'!$ABE$5,'Core Questionnaire'!$ACK$5,'Core Questionnaire'!$ADQ$5,'Core Questionnaire'!$AIQ$5,'Core Questionnaire'!$AJW$5)*100</f>
+        <v>83.0745454545455</v>
+      </c>
+      <c r="H4" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$5,'Core Questionnaire'!$FX$5,'Companion Questionnaire'!$CG$5,'Companion Questionnaire'!$CE$5,'Core Questionnaire'!$HC$5,'Core Questionnaire'!$HE$5)*100</f>
+        <v>72.0316666666667</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="J4" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CE$5, 'Core Questionnaire'!$CG$5, 'Core Questionnaire'!$CY$5, 'Core Questionnaire'!$DC$5, 'Core Questionnaire'!$DE$5, 'Core Questionnaire'!$DI$5, 'Core Questionnaire'!$DO$5, 'Core Questionnaire'!$DU$5, 'Core Questionnaire'!$FV$5, 'Core Questionnaire'!$FZ$5, 'Core Questionnaire'!$GB$5, 'Core Questionnaire'!$GF$5, 'Core Questionnaire'!$GL$5, 'Core Questionnaire'!$GR$5, 'Core Questionnaire'!$HG$5, 'Core Questionnaire'!$ALK$5, 'Core Questionnaire'!$ALM$5, 'Core Questionnaire'!$ALO$5, 'Core Questionnaire'!$ALQ$5)*100</f>
+        <v>55.5333333333333</v>
+      </c>
+      <c r="K4" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CS$5,'Core Questionnaire'!$CU$5,'Core Questionnaire'!$AAG$5,'Core Questionnaire'!$AAR$5,'Companion Questionnaire'!$CL$5,'Core Questionnaire'!$CW$5,'Core Questionnaire'!$ALF$5)*100</f>
+        <v>76.1428571428571</v>
+      </c>
+      <c r="L4" s="35" t="n">
+        <v>71.1</v>
+      </c>
+      <c r="M4" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FN5,'Companion Questionnaire'!CE5,'Companion Questionnaire'!CJ5,'Companion Questionnaire'!CQ5)*100</f>
         <v>75</v>
       </c>
-      <c r="C4" s="35" t="n">
+      <c r="N4" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FP5,'Companion Questionnaire'!BF5,'Companion Questionnaire'!BI5,'Companion Questionnaire'!CG5,'Companion Questionnaire'!CN5,'Companion Questionnaire'!CS5)*100</f>
         <v>75.5983333333333</v>
       </c>
-      <c r="D4" s="35" t="n">
-        <v>71.1</v>
-      </c>
-      <c r="E4" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CS5,'Core Questionnaire'!CU5,'Core Questionnaire'!AAG5,'Core Questionnaire'!AAR5,'Companion Questionnaire'!CL5,'Core Questionnaire'!CW5,'Core Questionnaire'!ALF5)*100</f>
-        <v>76.1428571428571</v>
-      </c>
-      <c r="F4" s="34" t="s">
+      <c r="O4" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CC$5:$CG$5)*100</f>
+        <v>66.6666666666667</v>
+      </c>
+      <c r="P4" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="Q4" s="34" t="s">
+        <v>1264</v>
+      </c>
+      <c r="R4" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZW$5:$AAE$5)*100</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="T4" s="34" t="s">
         <v>1261</v>
       </c>
-      <c r="G4" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZM5:ZU5,'Core Questionnaire'!AAI5:AAM5)*100</f>
-        <v>100</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="J4" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="K4" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZW5:AAE5)*100</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CC5:CG5)*100</f>
-        <v>66.6666666666667</v>
-      </c>
-      <c r="M4" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>1264</v>
-      </c>
-      <c r="O4" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA5,'Core Questionnaire'!FX5,'Core Questionnaire'!HC5,'Companion Questionnaire'!CE5,'Core Questionnaire'!HP5,'Core Questionnaire'!MP5,'Core Questionnaire'!PG5,'Core Questionnaire'!UE5,'Companion Questionnaire'!CG5,'Core Questionnaire'!HE5,'Core Questionnaire'!ABE5,'Core Questionnaire'!ACK5,'Core Questionnaire'!ADQ5,'Core Questionnaire'!AIQ5,'Core Questionnaire'!AJW5)*100</f>
-        <v>83.0745454545455</v>
-      </c>
-      <c r="P4" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA5,'Core Questionnaire'!FX5,'Companion Questionnaire'!CG5,'Companion Questionnaire'!CE5,'Core Questionnaire'!HC5,'Core Questionnaire'!HE5)*100</f>
-        <v>72.0316666666667</v>
-      </c>
-      <c r="Q4" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="R4" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CE5, 'Core Questionnaire'!CG5, 'Core Questionnaire'!CY5, 'Core Questionnaire'!DC5, 'Core Questionnaire'!DE5, 'Core Questionnaire'!DI5, 'Core Questionnaire'!DO5, 'Core Questionnaire'!DU5, 'Core Questionnaire'!FV5, 'Core Questionnaire'!FZ5, 'Core Questionnaire'!GB5, 'Core Questionnaire'!GF5, 'Core Questionnaire'!GL5, 'Core Questionnaire'!GR5, 'Core Questionnaire'!HG5, 'Core Questionnaire'!ALK5, 'Core Questionnaire'!ALM5, 'Core Questionnaire'!ALO5, 'Core Questionnaire'!ALQ5)*100</f>
-        <v>55.5333333333333</v>
-      </c>
-      <c r="S4" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DQ5,'Core Questionnaire'!GN5,'Core Questionnaire'!ALD5,'Core Questionnaire'!ALF5,'Companion Questionnaire'!BX5)*100</f>
-        <v>68.4</v>
-      </c>
-      <c r="T4" s="34" t="s">
-        <v>1262</v>
-      </c>
       <c r="U4" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="V4" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="W4" s="34" t="s">
         <v>1263</v>
       </c>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="35"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
         <v>1069</v>
       </c>
       <c r="B5" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DQ$6,'Core Questionnaire'!$GN$6,'Core Questionnaire'!$ALD$6,'Core Questionnaire'!$ALF$6,'Companion Questionnaire'!$BX$6)*100</f>
+        <v>58.25</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E5" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZM$6:$ZU$6,'Core Questionnaire'!$AAI$6:$AAM$6)*100</f>
+        <v>100</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="G5" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$6,'Core Questionnaire'!$FX$6,'Core Questionnaire'!$HC$6,'Companion Questionnaire'!$CE$6,'Core Questionnaire'!$HP$6,'Core Questionnaire'!$MP$6,'Core Questionnaire'!$PG$6,'Core Questionnaire'!$UE$6,'Companion Questionnaire'!$CG$6,'Core Questionnaire'!$HE$6,'Core Questionnaire'!$ABE$6,'Core Questionnaire'!$ACK$6,'Core Questionnaire'!$ADQ$6,'Core Questionnaire'!$AIQ$6,'Core Questionnaire'!$AJW$6)*100</f>
+        <v>67.5463636363637</v>
+      </c>
+      <c r="H5" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$6,'Core Questionnaire'!$FX$6,'Companion Questionnaire'!$CG$6,'Companion Questionnaire'!$CE$6,'Core Questionnaire'!$HC$6,'Core Questionnaire'!$HE$6)*100</f>
+        <v>64</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="J5" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CE$6, 'Core Questionnaire'!$CG$6, 'Core Questionnaire'!$CY$6, 'Core Questionnaire'!$DC$6, 'Core Questionnaire'!$DE$6, 'Core Questionnaire'!$DI$6, 'Core Questionnaire'!$DO$6, 'Core Questionnaire'!$DU$6, 'Core Questionnaire'!$FV$6, 'Core Questionnaire'!$FZ$6, 'Core Questionnaire'!$GB$6, 'Core Questionnaire'!$GF$6, 'Core Questionnaire'!$GL$6, 'Core Questionnaire'!$GR$6, 'Core Questionnaire'!$HG$6, 'Core Questionnaire'!$ALK$6, 'Core Questionnaire'!$ALM$6, 'Core Questionnaire'!$ALO$6, 'Core Questionnaire'!$ALQ$6)*100</f>
+        <v>82.1222222222222</v>
+      </c>
+      <c r="K5" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CS$6,'Core Questionnaire'!$CU$6,'Core Questionnaire'!$AAG$6,'Core Questionnaire'!$AAR$6,'Companion Questionnaire'!$CL$6,'Core Questionnaire'!$CW$6,'Core Questionnaire'!$ALF$6)*100</f>
+        <v>90.4285714285714</v>
+      </c>
+      <c r="L5" s="35" t="n">
+        <v>84.94</v>
+      </c>
+      <c r="M5" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FN6,'Companion Questionnaire'!CE6,'Companion Questionnaire'!CJ6,'Companion Questionnaire'!CQ6)*100</f>
         <v>100</v>
       </c>
-      <c r="C5" s="35" t="n">
+      <c r="N5" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FP6,'Companion Questionnaire'!BF6,'Companion Questionnaire'!BI6,'Companion Questionnaire'!CG6,'Companion Questionnaire'!CN6,'Companion Questionnaire'!CS6)*100</f>
         <v>62.94</v>
       </c>
-      <c r="D5" s="35" t="n">
-        <v>84.94</v>
-      </c>
-      <c r="E5" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CS6,'Core Questionnaire'!CU6,'Core Questionnaire'!AAG6,'Core Questionnaire'!AAR6,'Companion Questionnaire'!CL6,'Core Questionnaire'!CW6,'Core Questionnaire'!ALF6)*100</f>
-        <v>90.4285714285714</v>
-      </c>
-      <c r="F5" s="34" t="s">
+      <c r="O5" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CC$6:$CG$6)*100</f>
+        <v>100</v>
+      </c>
+      <c r="P5" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>1059</v>
+      </c>
+      <c r="R5" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZW$6:$AAE$6)*100</f>
+        <v>100</v>
+      </c>
+      <c r="S5" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="T5" s="34" t="s">
         <v>1261</v>
       </c>
-      <c r="G5" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZM6:ZU6,'Core Questionnaire'!AAI6:AAM6)*100</f>
-        <v>100</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="I5" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="K5" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZW6:AAE6)*100</f>
-        <v>100</v>
-      </c>
-      <c r="L5" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CC6:CG6)*100</f>
-        <v>100</v>
-      </c>
-      <c r="M5" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="N5" s="34" t="s">
-        <v>1059</v>
-      </c>
-      <c r="O5" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA6,'Core Questionnaire'!FX6,'Core Questionnaire'!HC6,'Companion Questionnaire'!CE6,'Core Questionnaire'!HP6,'Core Questionnaire'!MP6,'Core Questionnaire'!PG6,'Core Questionnaire'!UE6,'Companion Questionnaire'!CG6,'Core Questionnaire'!HE6,'Core Questionnaire'!ABE6,'Core Questionnaire'!ACK6,'Core Questionnaire'!ADQ6,'Core Questionnaire'!AIQ6,'Core Questionnaire'!AJW6)*100</f>
-        <v>67.5463636363636</v>
-      </c>
-      <c r="P5" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA6,'Core Questionnaire'!FX6,'Companion Questionnaire'!CG6,'Companion Questionnaire'!CE6,'Core Questionnaire'!HC6,'Core Questionnaire'!HE6)*100</f>
-        <v>64</v>
-      </c>
-      <c r="Q5" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="R5" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CE6, 'Core Questionnaire'!CG6, 'Core Questionnaire'!CY6, 'Core Questionnaire'!DC6, 'Core Questionnaire'!DE6, 'Core Questionnaire'!DI6, 'Core Questionnaire'!DO6, 'Core Questionnaire'!DU6, 'Core Questionnaire'!FV6, 'Core Questionnaire'!FZ6, 'Core Questionnaire'!GB6, 'Core Questionnaire'!GF6, 'Core Questionnaire'!GL6, 'Core Questionnaire'!GR6, 'Core Questionnaire'!HG6, 'Core Questionnaire'!ALK6, 'Core Questionnaire'!ALM6, 'Core Questionnaire'!ALO6, 'Core Questionnaire'!ALQ6)*100</f>
-        <v>82.1222222222222</v>
-      </c>
-      <c r="S5" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DQ6,'Core Questionnaire'!GN6,'Core Questionnaire'!ALD6,'Core Questionnaire'!ALF6,'Companion Questionnaire'!BX6)*100</f>
-        <v>58.25</v>
-      </c>
-      <c r="T5" s="34" t="s">
-        <v>1262</v>
-      </c>
       <c r="U5" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="V5" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="W5" s="34" t="s">
         <v>1263</v>
       </c>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="35"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
         <v>1072</v>
       </c>
       <c r="B6" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DQ$7,'Core Questionnaire'!$GN$7,'Core Questionnaire'!$ALD$7,'Core Questionnaire'!$ALF$7,'Companion Questionnaire'!$BX$7)*100</f>
+        <v>73.272</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E6" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZM$7:$ZU$7,'Core Questionnaire'!$AAI$7:$AAM$7)*100</f>
+        <v>100</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H6" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$7,'Core Questionnaire'!$FX$7,'Companion Questionnaire'!$CG$7,'Companion Questionnaire'!$CE$7,'Core Questionnaire'!$HC$7,'Core Questionnaire'!$HE$7)*100</f>
+        <v>91.8333333333333</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="J6" s="35" t="n">
+        <v>82.12</v>
+      </c>
+      <c r="K6" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CS$7,'Core Questionnaire'!$CU$7,'Core Questionnaire'!$AAG$7,'Core Questionnaire'!$AAR$7,'Companion Questionnaire'!$CL$7,'Core Questionnaire'!$CW$7,'Core Questionnaire'!$ALF$7)*100</f>
+        <v>95.1428571428571</v>
+      </c>
+      <c r="L6" s="35" t="n">
+        <v>95.81</v>
+      </c>
+      <c r="M6" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FN7,'Companion Questionnaire'!CE7,'Companion Questionnaire'!CJ7,'Companion Questionnaire'!CQ7)*100</f>
         <v>100</v>
       </c>
-      <c r="C6" s="35" t="n">
+      <c r="N6" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FP7,'Companion Questionnaire'!BF7,'Companion Questionnaire'!BI7,'Companion Questionnaire'!CG7,'Companion Questionnaire'!CN7,'Companion Questionnaire'!CS7)*100</f>
         <v>73.2666666666667</v>
       </c>
-      <c r="D6" s="35" t="n">
-        <v>95.81</v>
-      </c>
-      <c r="E6" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CS7,'Core Questionnaire'!CU7,'Core Questionnaire'!AAG7,'Core Questionnaire'!AAR7,'Companion Questionnaire'!CL7,'Core Questionnaire'!CW7,'Core Questionnaire'!ALF7)*100</f>
-        <v>95.1428571428571</v>
-      </c>
-      <c r="F6" s="34" t="s">
+      <c r="O6" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CC$7:$CG$7)*100</f>
+        <v>100</v>
+      </c>
+      <c r="P6" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="Q6" s="34" t="s">
+        <v>1264</v>
+      </c>
+      <c r="R6" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZW$7:$AAE$7)*100</f>
+        <v>100</v>
+      </c>
+      <c r="S6" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="T6" s="34" t="s">
         <v>1261</v>
       </c>
-      <c r="G6" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZM7:ZU7,'Core Questionnaire'!AAI7:AAM7)*100</f>
-        <v>100</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="J6" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="K6" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZW7:AAE7)*100</f>
-        <v>100</v>
-      </c>
-      <c r="L6" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CC7:CG7)*100</f>
-        <v>100</v>
-      </c>
-      <c r="M6" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="N6" s="34" t="s">
-        <v>1264</v>
-      </c>
-      <c r="O6" s="36" t="s">
-        <v>1059</v>
-      </c>
-      <c r="P6" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA7,'Core Questionnaire'!FX7,'Companion Questionnaire'!CG7,'Companion Questionnaire'!CE7,'Core Questionnaire'!HC7,'Core Questionnaire'!HE7)*100</f>
-        <v>91.8333333333333</v>
-      </c>
-      <c r="Q6" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="R6" s="35" t="n">
-        <v>82.12</v>
-      </c>
-      <c r="S6" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DQ7,'Core Questionnaire'!GN7,'Core Questionnaire'!ALD7,'Core Questionnaire'!ALF7,'Companion Questionnaire'!BX7)*100</f>
-        <v>73.272</v>
-      </c>
-      <c r="T6" s="34" t="s">
-        <v>1262</v>
-      </c>
       <c r="U6" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="V6" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="W6" s="34" t="s">
         <v>1263</v>
       </c>
+      <c r="X6" s="0"/>
+      <c r="Y6" s="0"/>
+      <c r="Z6" s="0"/>
+      <c r="AA6" s="0"/>
+      <c r="AB6" s="0"/>
+      <c r="AC6" s="0"/>
+      <c r="AD6" s="0"/>
+      <c r="AE6" s="35"/>
+      <c r="AH6" s="0"/>
+      <c r="AI6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
         <v>1075</v>
       </c>
       <c r="B7" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DQ$8,'Core Questionnaire'!$GN$8,'Core Questionnaire'!$ALD$8,'Core Questionnaire'!$ALF$8,'Companion Questionnaire'!$BX$8)*100</f>
+        <v>83.25</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E7" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZM$8:$ZU$8,'Core Questionnaire'!$AAI$8:$AAM$8)*100</f>
+        <v>100</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="G7" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$8,'Core Questionnaire'!$FX$8,'Core Questionnaire'!$HC$8,'Companion Questionnaire'!$CE$8,'Core Questionnaire'!$HP$8,'Core Questionnaire'!$MP$8,'Core Questionnaire'!$PG$8,'Core Questionnaire'!$UE$8,'Companion Questionnaire'!$CG$8,'Core Questionnaire'!$HE$8,'Core Questionnaire'!$ABE$8,'Core Questionnaire'!$ACK$8,'Core Questionnaire'!$ADQ$8,'Core Questionnaire'!$AIQ$8,'Core Questionnaire'!$AJW$8)*100</f>
+        <v>63.1775</v>
+      </c>
+      <c r="H7" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$8,'Core Questionnaire'!$FX$8,'Companion Questionnaire'!$CG$8,'Companion Questionnaire'!$CE$8,'Core Questionnaire'!$HC$8,'Core Questionnaire'!$HE$8)*100</f>
+        <v>43.6833333333333</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="J7" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CE$8, 'Core Questionnaire'!$CG$8, 'Core Questionnaire'!$CY$8, 'Core Questionnaire'!$DC$8, 'Core Questionnaire'!$DE$8, 'Core Questionnaire'!$DI$8, 'Core Questionnaire'!$DO$8, 'Core Questionnaire'!$DU$8, 'Core Questionnaire'!$FV$8, 'Core Questionnaire'!$FZ$8, 'Core Questionnaire'!$GB$8, 'Core Questionnaire'!$GF$8, 'Core Questionnaire'!$GL$8, 'Core Questionnaire'!$GR$8, 'Core Questionnaire'!$HG$8, 'Core Questionnaire'!$ALK$8, 'Core Questionnaire'!$ALM$8, 'Core Questionnaire'!$ALO$8, 'Core Questionnaire'!$ALQ$8)*100</f>
+        <v>52.6315789473684</v>
+      </c>
+      <c r="K7" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CS$8,'Core Questionnaire'!$CU$8,'Core Questionnaire'!$AAG$8,'Core Questionnaire'!$AAR$8,'Companion Questionnaire'!$CL$8,'Core Questionnaire'!$CW$8,'Core Questionnaire'!$ALF$8)*100</f>
+        <v>90.4285714285714</v>
+      </c>
+      <c r="L7" s="35" t="n">
+        <v>72.03</v>
+      </c>
+      <c r="M7" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FN8,'Companion Questionnaire'!CE8,'Companion Questionnaire'!CJ8,'Companion Questionnaire'!CQ8)*100</f>
         <v>75</v>
       </c>
-      <c r="C7" s="35" t="n">
+      <c r="N7" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FP8,'Companion Questionnaire'!BF8,'Companion Questionnaire'!BI8,'Companion Questionnaire'!CG8,'Companion Questionnaire'!CN8,'Companion Questionnaire'!CS8)*100</f>
         <v>72.5366666666667</v>
       </c>
-      <c r="D7" s="35" t="n">
-        <v>72.03</v>
-      </c>
-      <c r="E7" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CS8,'Core Questionnaire'!CU8,'Core Questionnaire'!AAG8,'Core Questionnaire'!AAR8,'Companion Questionnaire'!CL8,'Core Questionnaire'!CW8,'Core Questionnaire'!ALF8)*100</f>
-        <v>90.4285714285714</v>
-      </c>
-      <c r="F7" s="34" t="s">
+      <c r="O7" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CC$8:$CG$8)*100</f>
+        <v>100</v>
+      </c>
+      <c r="P7" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>1264</v>
+      </c>
+      <c r="R7" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZW$8:$AAE$8)*100</f>
+        <v>100</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="T7" s="34" t="s">
         <v>1261</v>
       </c>
-      <c r="G7" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZM8:ZU8,'Core Questionnaire'!AAI8:AAM8)*100</f>
-        <v>100</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="J7" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="K7" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZW8:AAE8)*100</f>
-        <v>100</v>
-      </c>
-      <c r="L7" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CC8:CG8)*100</f>
-        <v>100</v>
-      </c>
-      <c r="M7" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="N7" s="34" t="s">
-        <v>1264</v>
-      </c>
-      <c r="O7" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA8,'Core Questionnaire'!FX8,'Core Questionnaire'!HC8,'Companion Questionnaire'!CE8,'Core Questionnaire'!HP8,'Core Questionnaire'!MP8,'Core Questionnaire'!PG8,'Core Questionnaire'!UE8,'Companion Questionnaire'!CG8,'Core Questionnaire'!HE8,'Core Questionnaire'!ABE8,'Core Questionnaire'!ACK8,'Core Questionnaire'!ADQ8,'Core Questionnaire'!AIQ8,'Core Questionnaire'!AJW8)*100</f>
-        <v>63.1775</v>
-      </c>
-      <c r="P7" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA8,'Core Questionnaire'!FX8,'Companion Questionnaire'!CG8,'Companion Questionnaire'!CE8,'Core Questionnaire'!HC8,'Core Questionnaire'!HE8)*100</f>
-        <v>43.6833333333333</v>
-      </c>
-      <c r="Q7" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="R7" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CE8, 'Core Questionnaire'!CG8, 'Core Questionnaire'!CY8, 'Core Questionnaire'!DC8, 'Core Questionnaire'!DE8, 'Core Questionnaire'!DI8, 'Core Questionnaire'!DO8, 'Core Questionnaire'!DU8, 'Core Questionnaire'!FV8, 'Core Questionnaire'!FZ8, 'Core Questionnaire'!GB8, 'Core Questionnaire'!GF8, 'Core Questionnaire'!GL8, 'Core Questionnaire'!GR8, 'Core Questionnaire'!HG8, 'Core Questionnaire'!ALK8, 'Core Questionnaire'!ALM8, 'Core Questionnaire'!ALO8, 'Core Questionnaire'!ALQ8)*100</f>
-        <v>52.6315789473684</v>
-      </c>
-      <c r="S7" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DQ8,'Core Questionnaire'!GN8,'Core Questionnaire'!ALD8,'Core Questionnaire'!ALF8,'Companion Questionnaire'!BX8)*100</f>
-        <v>83.25</v>
-      </c>
-      <c r="T7" s="34" t="s">
-        <v>1262</v>
-      </c>
       <c r="U7" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="V7" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="W7" s="34" t="s">
         <v>1263</v>
       </c>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="35"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
         <v>1079</v>
       </c>
       <c r="B8" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DQ$9,'Core Questionnaire'!$GN$9,'Core Questionnaire'!$ALD$9,'Core Questionnaire'!$ALF$9,'Companion Questionnaire'!$BX$9)*100</f>
+        <v>58.25</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E8" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZM$9:$ZU$9,'Core Questionnaire'!$AAI$9:$AAM$9)*100</f>
+        <v>100</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="G8" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$9,'Core Questionnaire'!$FX$9,'Core Questionnaire'!$HC$9,'Companion Questionnaire'!$CE$9,'Core Questionnaire'!$HP$9,'Core Questionnaire'!$MP$9,'Core Questionnaire'!$PG$9,'Core Questionnaire'!$UE$9,'Companion Questionnaire'!$CG$9,'Core Questionnaire'!$HE$9,'Core Questionnaire'!$ABE$9,'Core Questionnaire'!$ACK$9,'Core Questionnaire'!$ADQ$9,'Core Questionnaire'!$AIQ$9,'Core Questionnaire'!$AJW$9)*100</f>
+        <v>82.0308333333333</v>
+      </c>
+      <c r="H8" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$DA$9,'Core Questionnaire'!$FX$9,'Companion Questionnaire'!$CG$9,'Companion Questionnaire'!$CE$9,'Core Questionnaire'!$HC$9,'Core Questionnaire'!$HE$9)*100</f>
+        <v>79.25</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="J8" s="35" t="n">
+        <v>50</v>
+      </c>
+      <c r="K8" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CS$9,'Core Questionnaire'!$CU$9,'Core Questionnaire'!$AAG$9,'Core Questionnaire'!$AAR$9,'Companion Questionnaire'!$CL$9,'Core Questionnaire'!$CW$9,'Core Questionnaire'!$ALF$9)*100</f>
+        <v>79.7142857142857</v>
+      </c>
+      <c r="L8" s="35" t="n">
+        <v>74.45</v>
+      </c>
+      <c r="M8" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FN9,'Companion Questionnaire'!CE9,'Companion Questionnaire'!CJ9,'Companion Questionnaire'!CQ9)*100</f>
         <v>62.5</v>
       </c>
-      <c r="C8" s="35" t="n">
+      <c r="N8" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!FP9,'Companion Questionnaire'!BF9,'Companion Questionnaire'!BI9,'Companion Questionnaire'!CG9,'Companion Questionnaire'!CN9,'Companion Questionnaire'!CS9)*100</f>
         <v>77.1933333333333</v>
       </c>
-      <c r="D8" s="35" t="n">
-        <v>74.45</v>
-      </c>
-      <c r="E8" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CS9,'Core Questionnaire'!CU9,'Core Questionnaire'!AAG9,'Core Questionnaire'!AAR9,'Companion Questionnaire'!CL9,'Core Questionnaire'!CW9,'Core Questionnaire'!ALF9)*100</f>
-        <v>79.7142857142857</v>
-      </c>
-      <c r="F8" s="34" t="s">
+      <c r="O8" s="35" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$CC$9:$CG$9)*100</f>
+        <v>100</v>
+      </c>
+      <c r="P8" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="Q8" s="34" t="s">
+        <v>1264</v>
+      </c>
+      <c r="R8" s="34" t="n">
+        <f aca="false">AVERAGE('Core Questionnaire'!$ZW$9:$AAE$9)*100</f>
+        <v>100</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>1263</v>
+      </c>
+      <c r="T8" s="34" t="s">
         <v>1261</v>
       </c>
-      <c r="G8" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZM9:ZU9,'Core Questionnaire'!AAI9:AAM9)*100</f>
-        <v>100</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>1262</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="K8" s="34" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!ZW9:AAE9)*100</f>
-        <v>100</v>
-      </c>
-      <c r="L8" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!CC9:CG9)*100</f>
-        <v>100</v>
-      </c>
-      <c r="M8" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="N8" s="34" t="s">
-        <v>1264</v>
-      </c>
-      <c r="O8" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA9,'Core Questionnaire'!FX9,'Core Questionnaire'!HC9,'Companion Questionnaire'!CE9,'Core Questionnaire'!HP9,'Core Questionnaire'!MP9,'Core Questionnaire'!PG9,'Core Questionnaire'!UE9,'Companion Questionnaire'!CG9,'Core Questionnaire'!HE9,'Core Questionnaire'!ABE9,'Core Questionnaire'!ACK9,'Core Questionnaire'!ADQ9,'Core Questionnaire'!AIQ9,'Core Questionnaire'!AJW9)*100</f>
-        <v>82.0308333333333</v>
-      </c>
-      <c r="P8" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DA9,'Core Questionnaire'!FX9,'Companion Questionnaire'!CG9,'Companion Questionnaire'!CE9,'Core Questionnaire'!HC9,'Core Questionnaire'!HE9)*100</f>
-        <v>79.25</v>
-      </c>
-      <c r="Q8" s="34" t="s">
-        <v>1263</v>
-      </c>
-      <c r="R8" s="35" t="n">
-        <v>50</v>
-      </c>
-      <c r="S8" s="35" t="n">
-        <f aca="false">AVERAGE('Core Questionnaire'!DQ9,'Core Questionnaire'!GN9,'Core Questionnaire'!ALD9,'Core Questionnaire'!ALF9,'Companion Questionnaire'!BX9)*100</f>
-        <v>58.25</v>
-      </c>
-      <c r="T8" s="34" t="s">
-        <v>1262</v>
-      </c>
       <c r="U8" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="V8" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="W8" s="34" t="s">
         <v>1263</v>
       </c>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="35"/>
+      <c r="AH8" s="0"/>
+      <c r="AI8" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fix bad code in original data
1.4.4.e -> 1.4.4e

Also added an exception to handle the case
</commit_message>
<xml_diff>
--- a/data/rtei_data_2015.xlsx
+++ b/data/rtei_data_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="551" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="551" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Core Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
@@ -554,7 +554,7 @@
     <t>1.4.4e: Political or other opinion</t>
   </si>
   <si>
-    <t>1.4.4.e: Response</t>
+    <t>1.4.4e: Response</t>
   </si>
   <si>
     <t>1.4.4f: National or social origin</t>
@@ -4546,7 +4546,281 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4f81bd"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$B$19:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c0504d"/>
+            </a:solidFill>
+            <a:ln w="25560">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]'Private Education'!$E$19:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="15538815"/>
+        <c:axId val="94810994"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="15538815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>School Level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="94810994"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="94810994"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Gross Enrollment Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="15538815"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4686,11 +4960,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="22352211"/>
-        <c:axId val="86315210"/>
+        <c:axId val="84588139"/>
+        <c:axId val="82090845"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="22352211"/>
+        <c:axId val="84588139"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4730,14 +5004,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="86315210"/>
+        <c:crossAx val="82090845"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86315210"/>
+        <c:axId val="82090845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4784,7 +5058,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22352211"/>
+        <c:crossAx val="84588139"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4820,7 +5094,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4960,11 +5234,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="34804857"/>
-        <c:axId val="22661935"/>
+        <c:axId val="3263938"/>
+        <c:axId val="15178117"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="34804857"/>
+        <c:axId val="3263938"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5004,14 +5278,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22661935"/>
+        <c:crossAx val="15178117"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22661935"/>
+        <c:axId val="15178117"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5058,7 +5332,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="34804857"/>
+        <c:crossAx val="3263938"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5094,7 +5368,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5222,11 +5496,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="27788400"/>
-        <c:axId val="46336699"/>
+        <c:axId val="6938328"/>
+        <c:axId val="5375010"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="27788400"/>
+        <c:axId val="6938328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5266,14 +5540,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46336699"/>
+        <c:crossAx val="5375010"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46336699"/>
+        <c:axId val="5375010"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5320,281 +5594,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27788400"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4f81bd"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$B$19:$D$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0504d"/>
-            </a:solidFill>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]'Private Education'!$A$28:$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]'Private Education'!$E$19:$G$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="57373275"/>
-        <c:axId val="19104153"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="57373275"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>School Level</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="19104153"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="19104153"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Gross Enrollment Rate</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="57373275"/>
+        <c:crossAx val="6938328"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5785,10 +5785,10 @@
   </sheetPr>
   <dimension ref="A1:AMF11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="AKY1" activePane="topRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="DH1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="ALB11" activeCellId="0" sqref="ALB11"/>
+      <selection pane="topRight" activeCell="DH4" activeCellId="0" sqref="DH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25334,8 +25334,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X16" activeCellId="0" sqref="X16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Separate codes with colons instead of points in Tranversal Themes Mappings
</commit_message>
<xml_diff>
--- a/data/rtei_data_2015.xlsx
+++ b/data/rtei_data_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="551" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="656" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Core Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1357">
   <si>
     <t>Theme</t>
   </si>
@@ -3827,67 +3827,10 @@
     <t>Level 1: Category</t>
   </si>
   <si>
-    <t>1. Children with Disabilities</t>
-  </si>
-  <si>
-    <t>2. Content of Education</t>
-  </si>
-  <si>
-    <t>3. Girls' Education</t>
-  </si>
-  <si>
-    <t>4. Indigenous and Minority Populations</t>
-  </si>
-  <si>
-    <t>5. Monitoring and Accountability</t>
-  </si>
-  <si>
-    <t>6. National Normative Framework</t>
-  </si>
-  <si>
-    <t>7. Opportunity and Indirect Costs</t>
-  </si>
-  <si>
-    <t>8. Private Education</t>
-  </si>
-  <si>
-    <t>9. Teachers</t>
-  </si>
-  <si>
     <t>Level 2: Transversal Theme</t>
   </si>
   <si>
-    <t>1A. Structure and support </t>
-  </si>
-  <si>
-    <t>2A. Content of curriculum</t>
-  </si>
-  <si>
-    <t>3A. Overall state of girls' education</t>
-  </si>
-  <si>
-    <t>3B. Discriminatory environment</t>
-  </si>
-  <si>
-    <t>4A. Discriminatory environment</t>
-  </si>
-  <si>
-    <t>5A. Strength of monitoring and accountability</t>
-  </si>
-  <si>
-    <t>6A. National Normative Framework</t>
-  </si>
-  <si>
-    <t>7A. Legal restrictions in opportunity and indirect costs</t>
-  </si>
-  <si>
-    <t>7B. Opportunity and indirect costs in practice</t>
-  </si>
-  <si>
-    <t>8A. Private education legal environment</t>
-  </si>
-  <si>
-    <t>9A. Content of teacher training</t>
+    <t>1A: Structure and support</t>
   </si>
   <si>
     <t>Level 3: Indicators</t>
@@ -3905,10 +3848,7 @@
     <t>1.2.4: Do national laws protect the rights of minorities to establish private schools?</t>
   </si>
   <si>
-    <t>1.2.1a: Do national laws protect the right to primary education? </t>
-  </si>
-  <si>
-    <t>3.1.4a - Are tuition fees charged for public university/higher education in 2014?</t>
+    <t>3.1.4a: Are tuition fees charged for public university/higher education in 2014?</t>
   </si>
   <si>
     <t>4.1.3a: Does the required training for teachers include improving the skills necessary for teaching towards the full development of the child’s personality, talents, and mental and physical abilities?</t>
@@ -3926,9 +3866,6 @@
     <t>5.4.1a: Does national law prohibit early marriage (below the age of 18)?</t>
   </si>
   <si>
-    <t>3.1.2 - What percent of household spending was spent on primary education in 2013?</t>
-  </si>
-  <si>
     <t>4.1.3b: Does the required training for teachers include improving the skills necessary for teaching towards the full development of respect for human rights and fundamental freedoms?</t>
   </si>
   <si>
@@ -3953,7 +3890,7 @@
     <t>5.4.2: Is the legal minimum age of employment 15 or above?</t>
   </si>
   <si>
-    <t>3.1.3 - What percent of household spending was spent on secondary education in 2013?</t>
+    <t>3.1.3: What percent of household spending was spent on secondary education in 2013?</t>
   </si>
   <si>
     <t>4.1.3c: Does the required training for teachers include improving the skills necessary for teaching towards the full development of respect for the child’s parents, cultural identity, language, and values, as well as respect for the values of the child’s country and other civilizations?</t>
@@ -4546,7 +4483,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4686,11 +4623,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="15538815"/>
-        <c:axId val="94810994"/>
+        <c:axId val="29692189"/>
+        <c:axId val="49269088"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="15538815"/>
+        <c:axId val="29692189"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4730,14 +4667,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="94810994"/>
+        <c:crossAx val="49269088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94810994"/>
+        <c:axId val="49269088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4784,7 +4721,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15538815"/>
+        <c:crossAx val="29692189"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4820,7 +4757,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4960,11 +4897,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="84588139"/>
-        <c:axId val="82090845"/>
+        <c:axId val="93788246"/>
+        <c:axId val="90571939"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="84588139"/>
+        <c:axId val="93788246"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5004,14 +4941,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82090845"/>
+        <c:crossAx val="90571939"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82090845"/>
+        <c:axId val="90571939"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5058,7 +4995,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84588139"/>
+        <c:crossAx val="93788246"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5094,7 +5031,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5234,11 +5171,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="3263938"/>
-        <c:axId val="15178117"/>
+        <c:axId val="60434288"/>
+        <c:axId val="23056192"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="3263938"/>
+        <c:axId val="60434288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5278,14 +5215,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15178117"/>
+        <c:crossAx val="23056192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15178117"/>
+        <c:axId val="23056192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5332,7 +5269,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3263938"/>
+        <c:crossAx val="60434288"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5368,7 +5305,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5496,11 +5433,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="6938328"/>
-        <c:axId val="5375010"/>
+        <c:axId val="44933029"/>
+        <c:axId val="69313615"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="6938328"/>
+        <c:axId val="44933029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5540,14 +5477,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5375010"/>
+        <c:crossAx val="69313615"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5375010"/>
+        <c:axId val="69313615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5594,7 +5531,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="6938328"/>
+        <c:crossAx val="44933029"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5635,15 +5572,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1280880</xdr:colOff>
+      <xdr:colOff>1307880</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>320760</xdr:colOff>
+      <xdr:colOff>347400</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5651,8 +5588,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20000520" y="4269240"/>
-        <a:ext cx="5847120" cy="2513520"/>
+        <a:off x="20027520" y="4260240"/>
+        <a:ext cx="5846760" cy="2513160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5665,15 +5602,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>598320</xdr:colOff>
+      <xdr:colOff>625320</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>63720</xdr:colOff>
+      <xdr:colOff>90360</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5681,8 +5618,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26125200" y="4278600"/>
-        <a:ext cx="6272640" cy="2513520"/>
+        <a:off x="26152200" y="4269600"/>
+        <a:ext cx="6272280" cy="2513160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5695,15 +5632,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1280880</xdr:colOff>
+      <xdr:colOff>1307880</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>320760</xdr:colOff>
+      <xdr:colOff>347400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>64080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5711,8 +5648,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20000520" y="6898320"/>
-        <a:ext cx="5847120" cy="2513880"/>
+        <a:off x="20027520" y="6889320"/>
+        <a:ext cx="5846760" cy="2513520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5725,15 +5662,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>607680</xdr:colOff>
+      <xdr:colOff>634680</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>73080</xdr:colOff>
+      <xdr:colOff>99720</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>64080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5741,8 +5678,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26134560" y="6898320"/>
-        <a:ext cx="6272640" cy="2513880"/>
+        <a:off x="26161560" y="6889320"/>
+        <a:ext cx="6272280" cy="2513520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5785,7 +5722,7 @@
   </sheetPr>
   <dimension ref="A1:AMF11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="DH1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="DH4" activeCellId="0" sqref="DH4"/>
@@ -20358,8 +20295,8 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB6" activeCellId="0" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -20404,121 +20341,121 @@
         <v>1265</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1266</v>
+        <v>1227</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1267</v>
+        <v>1228</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1268</v>
+        <v>1229</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1269</v>
+        <v>1230</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1270</v>
+        <v>1231</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>1271</v>
+        <v>1232</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>1272</v>
+        <v>1233</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>1273</v>
+        <v>1234</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>1274</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1275</v>
+        <v>1266</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1276</v>
+        <v>1267</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1277</v>
+        <v>1242</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>1278</v>
+        <v>1244</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>1279</v>
+        <v>1245</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>1280</v>
+        <v>1247</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>1281</v>
+        <v>1248</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>1282</v>
+        <v>1249</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>1283</v>
+        <v>1250</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>1284</v>
+        <v>1251</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>1285</v>
+        <v>1252</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>1286</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1287</v>
+        <v>1268</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1288</v>
+        <v>1269</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>1289</v>
+        <v>1270</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>1290</v>
+        <v>1271</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>1290</v>
+        <v>1271</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>1291</v>
+        <v>1272</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>38</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>1292</v>
+        <v>145</v>
       </c>
       <c r="X3" s="0" t="s">
         <v>48</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>1293</v>
+        <v>1273</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>33</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>1294</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>1295</v>
+        <v>1275</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>1296</v>
+        <v>1276</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>1297</v>
+        <v>1277</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>1297</v>
+        <v>1277</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>35</v>
@@ -20530,149 +20467,149 @@
         <v>147</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>1298</v>
+        <v>1278</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>1299</v>
+        <v>49</v>
       </c>
       <c r="AC4" s="0" t="s">
         <v>34</v>
       </c>
       <c r="AF4" s="0" t="s">
-        <v>1300</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>1301</v>
+        <v>1280</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>1302</v>
+        <v>1281</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>1303</v>
+        <v>1282</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>1304</v>
+        <v>1283</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>1305</v>
+        <v>1284</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>61</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>1306</v>
+        <v>1285</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>1307</v>
+        <v>1286</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>1308</v>
+        <v>1287</v>
       </c>
       <c r="AC5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="AF5" s="0" t="s">
-        <v>1309</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>1310</v>
+        <v>1289</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>1311</v>
+        <v>1290</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>1304</v>
+        <v>1283</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>1303</v>
+        <v>1282</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>1312</v>
+        <v>1291</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>1313</v>
+        <v>1292</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>151</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>1314</v>
+        <v>1293</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>1315</v>
+        <v>1294</v>
       </c>
       <c r="AF6" s="0" t="s">
-        <v>1316</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>1317</v>
+        <v>1296</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>1318</v>
+        <v>1297</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>1319</v>
+        <v>1298</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>1315</v>
+        <v>1294</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>1320</v>
+        <v>1299</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>1321</v>
+        <v>1300</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>33</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>1322</v>
+        <v>1301</v>
       </c>
       <c r="AF7" s="0" t="s">
-        <v>1323</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="0" t="s">
-        <v>1324</v>
+        <v>1303</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>1325</v>
+        <v>1304</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>52</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>1326</v>
+        <v>1305</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>1327</v>
+        <v>1306</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>34</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>1328</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="0" t="s">
-        <v>1329</v>
+        <v>1308</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>1330</v>
+        <v>1309</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>1331</v>
+        <v>1310</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>1310</v>
+        <v>1289</v>
       </c>
       <c r="U9" s="0" t="s">
         <v>35</v>
@@ -20680,13 +20617,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="s">
-        <v>1332</v>
+        <v>1311</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>1333</v>
+        <v>1312</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>1334</v>
+        <v>1313</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>36</v>
@@ -20694,13 +20631,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>1314</v>
+      </c>
+      <c r="U11" s="0" t="s">
         <v>1315</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>1335</v>
-      </c>
-      <c r="U11" s="0" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20708,7 +20645,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>1337</v>
+        <v>1316</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>38</v>
@@ -20716,10 +20653,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="0" t="s">
-        <v>1338</v>
+        <v>1317</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>1339</v>
+        <v>1318</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>39</v>
@@ -20727,160 +20664,160 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J14" s="0" t="s">
-        <v>1340</v>
+        <v>1319</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>1341</v>
+        <v>1320</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>1342</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="0" t="s">
-        <v>1343</v>
+        <v>1322</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>1344</v>
+        <v>1323</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>1345</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="0" t="s">
-        <v>1346</v>
+        <v>1325</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>1347</v>
+        <v>1326</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>1348</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="0" t="s">
-        <v>1349</v>
+        <v>1328</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>53</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>1350</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O18" s="0" t="s">
-        <v>1351</v>
+        <v>1330</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>1352</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O19" s="0" t="s">
-        <v>1353</v>
+        <v>1332</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>1354</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O20" s="0" t="s">
-        <v>1355</v>
+        <v>1334</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>1356</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U21" s="0" t="s">
-        <v>1357</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U22" s="0" t="s">
-        <v>1358</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U23" s="0" t="s">
-        <v>1359</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U24" s="0" t="s">
-        <v>1360</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U25" s="0" t="s">
-        <v>1361</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U26" s="0" t="s">
-        <v>1362</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U27" s="0" t="s">
-        <v>1363</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U28" s="0" t="s">
-        <v>1364</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U29" s="0" t="s">
-        <v>1365</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U30" s="0" t="s">
-        <v>1366</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U31" s="0" t="s">
-        <v>1303</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U32" s="0" t="s">
-        <v>1367</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U33" s="0" t="s">
-        <v>1368</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U34" s="0" t="s">
-        <v>1369</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U35" s="0" t="s">
-        <v>1370</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U36" s="0" t="s">
-        <v>1371</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U37" s="0" t="s">
-        <v>1372</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U38" s="0" t="s">
-        <v>1313</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20890,57 +20827,57 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U40" s="0" t="s">
-        <v>1373</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U41" s="0" t="s">
-        <v>1353</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U42" s="0" t="s">
-        <v>1374</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U43" s="0" t="s">
-        <v>1375</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U44" s="0" t="s">
-        <v>1376</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U45" s="0" t="s">
-        <v>1377</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U46" s="0" t="s">
-        <v>1307</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U47" s="0" t="s">
-        <v>1321</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U48" s="0" t="s">
-        <v>1314</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U49" s="0" t="s">
-        <v>1327</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U50" s="0" t="s">
-        <v>1310</v>
+        <v>1289</v>
       </c>
     </row>
   </sheetData>
@@ -25348,6 +25285,12 @@
       <c r="A1" s="34" t="s">
         <v>1226</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
@@ -25387,6 +25330,7 @@
       <c r="E2" s="34" t="s">
         <v>1228</v>
       </c>
+      <c r="F2" s="0"/>
       <c r="G2" s="34" t="s">
         <v>1229</v>
       </c>
@@ -25413,6 +25357,7 @@
       <c r="R2" s="34" t="s">
         <v>1235</v>
       </c>
+      <c r="S2" s="0"/>
       <c r="T2" s="34" t="s">
         <v>1236</v>
       </c>
@@ -25430,6 +25375,7 @@
       <c r="AB2" s="0"/>
       <c r="AC2" s="0"/>
       <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
       <c r="AF2" s="0"/>
       <c r="AG2" s="0"/>
       <c r="AH2" s="0"/>
@@ -25510,6 +25456,7 @@
       <c r="AB3" s="0"/>
       <c r="AC3" s="0"/>
       <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
       <c r="AH3" s="0"/>
       <c r="AI3" s="0"/>
     </row>

</xml_diff>

<commit_message>
Update code for 1A to 1A.A pon Transversal Themes Mappings
</commit_message>
<xml_diff>
--- a/data/rtei_data_2015.xlsx
+++ b/data/rtei_data_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="656" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="408" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Core Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1356">
   <si>
     <t>Theme</t>
   </si>
@@ -3828,9 +3828,6 @@
   </si>
   <si>
     <t>Level 2: Transversal Theme</t>
-  </si>
-  <si>
-    <t>1A: Structure and support</t>
   </si>
   <si>
     <t>Level 3: Indicators</t>
@@ -4623,11 +4620,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="29692189"/>
-        <c:axId val="49269088"/>
+        <c:axId val="1232778"/>
+        <c:axId val="60918029"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="29692189"/>
+        <c:axId val="1232778"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4667,14 +4664,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49269088"/>
+        <c:crossAx val="60918029"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49269088"/>
+        <c:axId val="60918029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4721,7 +4718,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29692189"/>
+        <c:crossAx val="1232778"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4897,11 +4894,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="93788246"/>
-        <c:axId val="90571939"/>
+        <c:axId val="30536161"/>
+        <c:axId val="6569285"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="93788246"/>
+        <c:axId val="30536161"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4941,14 +4938,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="90571939"/>
+        <c:crossAx val="6569285"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90571939"/>
+        <c:axId val="6569285"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4995,7 +4992,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93788246"/>
+        <c:crossAx val="30536161"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5171,11 +5168,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60434288"/>
-        <c:axId val="23056192"/>
+        <c:axId val="90303621"/>
+        <c:axId val="30459267"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="60434288"/>
+        <c:axId val="90303621"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5215,14 +5212,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23056192"/>
+        <c:crossAx val="30459267"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23056192"/>
+        <c:axId val="30459267"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5269,7 +5266,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="60434288"/>
+        <c:crossAx val="90303621"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5433,11 +5430,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="44933029"/>
-        <c:axId val="69313615"/>
+        <c:axId val="98211591"/>
+        <c:axId val="98642708"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="44933029"/>
+        <c:axId val="98211591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5477,14 +5474,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69313615"/>
+        <c:crossAx val="98642708"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69313615"/>
+        <c:axId val="98642708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5531,7 +5528,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44933029"/>
+        <c:crossAx val="98211591"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5572,15 +5569,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1307880</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:colOff>1334880</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>347400</xdr:colOff>
+      <xdr:colOff>374040</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:rowOff>54000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5588,8 +5585,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20027520" y="4260240"/>
-        <a:ext cx="5846760" cy="2513160"/>
+        <a:off x="20054520" y="4251240"/>
+        <a:ext cx="5846400" cy="2512800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5602,15 +5599,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>625320</xdr:colOff>
+      <xdr:colOff>652320</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>90360</xdr:colOff>
+      <xdr:colOff>117000</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5618,8 +5615,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26152200" y="4269600"/>
-        <a:ext cx="6272280" cy="2513160"/>
+        <a:off x="26179200" y="4260600"/>
+        <a:ext cx="6271920" cy="2512800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5632,15 +5629,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1307880</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:colOff>1334880</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>347400</xdr:colOff>
+      <xdr:colOff>374040</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5648,8 +5645,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20027520" y="6889320"/>
-        <a:ext cx="5846760" cy="2513520"/>
+        <a:off x="20054520" y="6880320"/>
+        <a:ext cx="5846400" cy="2513160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5662,15 +5659,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>634680</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:colOff>661680</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>99720</xdr:colOff>
+      <xdr:colOff>126360</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5678,8 +5675,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26161560" y="6889320"/>
-        <a:ext cx="6272280" cy="2513520"/>
+        <a:off x="26188560" y="6880320"/>
+        <a:ext cx="6271920" cy="2513160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20295,8 +20292,8 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB6" activeCellId="0" sqref="AB6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -20373,7 +20370,7 @@
         <v>1266</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1267</v>
+        <v>1239</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>1242</v>
@@ -20408,22 +20405,22 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>1268</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>1269</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>1270</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="L3" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="O3" s="0" t="s">
         <v>1271</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>1271</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>1272</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>38</v>
@@ -20435,27 +20432,27 @@
         <v>48</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>33</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>1275</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>1276</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>1277</v>
-      </c>
       <c r="L4" s="0" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>35</v>
@@ -20467,7 +20464,7 @@
         <v>147</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>49</v>
@@ -20476,140 +20473,140 @@
         <v>34</v>
       </c>
       <c r="AF4" s="0" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>1280</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>1281</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="L5" s="0" t="s">
         <v>1282</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="O5" s="0" t="s">
         <v>1283</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>1284</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>61</v>
       </c>
       <c r="U5" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="X5" s="0" t="s">
         <v>1285</v>
       </c>
-      <c r="X5" s="0" t="s">
+      <c r="Z5" s="0" t="s">
         <v>1286</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>1287</v>
       </c>
       <c r="AC5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="AF5" s="0" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>1289</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="J6" s="0" t="s">
+        <v>1282</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="O6" s="0" t="s">
         <v>1290</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>1283</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>1282</v>
-      </c>
-      <c r="O6" s="0" t="s">
+      <c r="R6" s="0" t="s">
         <v>1291</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>1292</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>151</v>
       </c>
       <c r="X6" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="Z6" s="0" t="s">
         <v>1293</v>
       </c>
-      <c r="Z6" s="0" t="s">
+      <c r="AF6" s="0" t="s">
         <v>1294</v>
-      </c>
-      <c r="AF6" s="0" t="s">
-        <v>1295</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>1296</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>1297</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="L7" s="0" t="s">
+        <v>1293</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>1298</v>
       </c>
-      <c r="L7" s="0" t="s">
-        <v>1294</v>
-      </c>
-      <c r="O7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>1299</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>1300</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>33</v>
       </c>
       <c r="Z7" s="0" t="s">
+        <v>1300</v>
+      </c>
+      <c r="AF7" s="0" t="s">
         <v>1301</v>
-      </c>
-      <c r="AF7" s="0" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="0" t="s">
+        <v>1302</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>1303</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>1304</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>52</v>
       </c>
       <c r="O8" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="R8" s="0" t="s">
         <v>1305</v>
-      </c>
-      <c r="R8" s="0" t="s">
-        <v>1306</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>34</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>1308</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="O9" s="0" t="s">
         <v>1309</v>
       </c>
-      <c r="O9" s="0" t="s">
-        <v>1310</v>
-      </c>
       <c r="R9" s="0" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="U9" s="0" t="s">
         <v>35</v>
@@ -20617,13 +20614,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="s">
+        <v>1310</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>1311</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="O10" s="0" t="s">
         <v>1312</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>1313</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>36</v>
@@ -20631,13 +20628,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="0" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="O11" s="0" t="s">
+        <v>1313</v>
+      </c>
+      <c r="U11" s="0" t="s">
         <v>1314</v>
-      </c>
-      <c r="U11" s="0" t="s">
-        <v>1315</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20645,7 +20642,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>38</v>
@@ -20653,10 +20650,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="0" t="s">
+        <v>1316</v>
+      </c>
+      <c r="O13" s="0" t="s">
         <v>1317</v>
-      </c>
-      <c r="O13" s="0" t="s">
-        <v>1318</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>39</v>
@@ -20664,160 +20661,160 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J14" s="0" t="s">
+        <v>1318</v>
+      </c>
+      <c r="O14" s="0" t="s">
         <v>1319</v>
       </c>
-      <c r="O14" s="0" t="s">
+      <c r="U14" s="0" t="s">
         <v>1320</v>
-      </c>
-      <c r="U14" s="0" t="s">
-        <v>1321</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="0" t="s">
+        <v>1321</v>
+      </c>
+      <c r="O15" s="0" t="s">
         <v>1322</v>
       </c>
-      <c r="O15" s="0" t="s">
+      <c r="U15" s="0" t="s">
         <v>1323</v>
-      </c>
-      <c r="U15" s="0" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="0" t="s">
+        <v>1324</v>
+      </c>
+      <c r="O16" s="0" t="s">
         <v>1325</v>
       </c>
-      <c r="O16" s="0" t="s">
+      <c r="U16" s="0" t="s">
         <v>1326</v>
-      </c>
-      <c r="U16" s="0" t="s">
-        <v>1327</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="0" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>53</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O18" s="0" t="s">
+        <v>1329</v>
+      </c>
+      <c r="U18" s="0" t="s">
         <v>1330</v>
-      </c>
-      <c r="U18" s="0" t="s">
-        <v>1331</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O19" s="0" t="s">
+        <v>1331</v>
+      </c>
+      <c r="U19" s="0" t="s">
         <v>1332</v>
-      </c>
-      <c r="U19" s="0" t="s">
-        <v>1333</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O20" s="0" t="s">
+        <v>1333</v>
+      </c>
+      <c r="U20" s="0" t="s">
         <v>1334</v>
-      </c>
-      <c r="U20" s="0" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U21" s="0" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U22" s="0" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U23" s="0" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U24" s="0" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U25" s="0" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U26" s="0" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U27" s="0" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U28" s="0" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U29" s="0" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U30" s="0" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U31" s="0" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U32" s="0" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U33" s="0" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U34" s="0" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U35" s="0" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U36" s="0" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U37" s="0" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U38" s="0" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20827,57 +20824,57 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U40" s="0" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U41" s="0" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U42" s="0" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U43" s="0" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U44" s="0" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U45" s="0" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U46" s="0" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U47" s="0" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U48" s="0" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U49" s="0" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U50" s="0" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typos in original spreadsheet
</commit_message>
<xml_diff>
--- a/data/rtei_data_2015.xlsx
+++ b/data/rtei_data_2015.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1354">
   <si>
     <t>Theme</t>
   </si>
@@ -158,7 +158,7 @@
     <t>2.1.1: What is the pupil-classroom ratio?</t>
   </si>
   <si>
-    <t>2.2.1: What is th percentage of schools with toilets?</t>
+    <t>2.2.1: What is the percentage of schools with toilets?</t>
   </si>
   <si>
     <t>2.2.2: What is the percentage of schools with potable water?</t>
@@ -236,7 +236,7 @@
     <t>5.1.1: Do national laws recognize the right to education for children with disabilities?</t>
   </si>
   <si>
-    <t>5.1.2: Are reasonable accomodation measures available for children with disabilities in mainstream schools?</t>
+    <t>5.1.2: Are reasonable accommodation measures available for children with disabilities in mainstream schools?</t>
   </si>
   <si>
     <t>5.2.1: Are there mobile schools for children of nomads?</t>
@@ -254,10 +254,10 @@
     <t>5.3.2: Is education available in prison?</t>
   </si>
   <si>
-    <t>5.3.3: Do imprisoned children receive educatin integrated with the general education system (i.e., same curricula)?</t>
-  </si>
-  <si>
-    <t>5.3.4: Are children prisoners-of-war givent he means to pursue their educational activities?</t>
+    <t>5.3.3: Do imprisoned children receive education integrated with the general education system (i.e., same curricula)?</t>
+  </si>
+  <si>
+    <t>5.3.4: Are children prisoners-of-war given the means to pursue their educational activities?</t>
   </si>
   <si>
     <t>1.1.1a: The International Covenant of Economic, Social and Cultural Rights</t>
@@ -887,7 +887,7 @@
     <t>3.3.1ah: Response</t>
   </si>
   <si>
-    <t>3.3.1ai: Primay schools - Q4</t>
+    <t>3.3.1ai: Primary schools - Q4</t>
   </si>
   <si>
     <t>3.3.1ai: Response</t>
@@ -1277,7 +1277,7 @@
     <t>3.3.2ah: Response</t>
   </si>
   <si>
-    <t>3.3.2ai: Primay schools - Q4</t>
+    <t>3.3.2ai: Primary schools - Q4</t>
   </si>
   <si>
     <t>3.3.2ai: Response</t>
@@ -1346,7 +1346,7 @@
     <t>3.3.2bd: Secondary schools - urban</t>
   </si>
   <si>
-    <t>3.3.2bd: Resposne</t>
+    <t>3.3.2bd: Response</t>
   </si>
   <si>
     <t>3.3.2be: Secondary schools - rural</t>
@@ -1484,7 +1484,7 @@
     <t>3.3.4ah: Response</t>
   </si>
   <si>
-    <t>3.3.4ai: Public primay schools - Q4</t>
+    <t>3.3.4ai: Public primary schools - Q4</t>
   </si>
   <si>
     <t>3.3.4ai: Response</t>
@@ -1868,7 +1868,7 @@
     <t>3.3.4eh: Response</t>
   </si>
   <si>
-    <t>3.3.4ei: Private primay schools - Q4</t>
+    <t>3.3.4ei: Private primary schools - Q4</t>
   </si>
   <si>
     <t>3.3.4ei: Response</t>
@@ -3242,9 +3242,6 @@
     <t>Yes, and it is justiciable</t>
   </si>
   <si>
-    <t>Mising</t>
-  </si>
-  <si>
     <t>Philippines</t>
   </si>
   <si>
@@ -3323,7 +3320,7 @@
     <t>C 2.3.2: What is the pupil-trained teacher ratio?</t>
   </si>
   <si>
-    <t>C 2.3.3: What is the mean teacher slary relative to the national mean salary in 2014?</t>
+    <t>C 2.3.3: What is the mean teacher salary relative to the national mean salary in 2014?</t>
   </si>
   <si>
     <t>C 2.4.1: What is the pupil-textbook ratio?</t>
@@ -3332,7 +3329,7 @@
     <t>C 3.1.3: What percent of household spending was spent on secondary education in 2013?</t>
   </si>
   <si>
-    <t>C 3.1.4: Are tuition fees chared for public university/higher education?</t>
+    <t>C 3.1.4: Are tuition fees charged for public university/higher education?</t>
   </si>
   <si>
     <t>C 3.1.5: Is basic education publicly provided for adults who have not completed primary education?</t>
@@ -3341,7 +3338,7 @@
     <t>C 3.3.3: What is the share of private school enrollment?</t>
   </si>
   <si>
-    <t>C 4.1.6: Do national laws include children in the deciion making process of school curricula, school policies, and codes of behavior?</t>
+    <t>C 4.1.6: Do national laws include children in the decision making process of school curricula, school policies, and codes of behavior?</t>
   </si>
   <si>
     <t>C 5.1.3: What is the percentage of teachers trained to teach children with disabilities?</t>
@@ -3362,7 +3359,7 @@
     <t>C 5.4.4: In 2014, what percent of children under the age of 15 worked in the labor force?</t>
   </si>
   <si>
-    <t>C 5.4.5a: Is the legal minimum age of military rectuitment 15 or above?</t>
+    <t>C 5.4.5a: Is the legal minimum age of military recruitment 15 or above?</t>
   </si>
   <si>
     <t>C 5.4.5b: Are children under the age of 15 recruited by the military in practice?</t>
@@ -3458,7 +3455,7 @@
     <t>C 2.1.1: Response</t>
   </si>
   <si>
-    <t>C 2.1.1_yera</t>
+    <t>C 2.1.1_year</t>
   </si>
   <si>
     <t>C 2.2.1: What is the percentage of secondary schools with toilets in 2014?</t>
@@ -3527,7 +3524,7 @@
     <t>C 3.1.3_year</t>
   </si>
   <si>
-    <t>C 3.1.4a: Are tuition fees chared for public university/higher education in 2014?</t>
+    <t>C 3.1.4a: Are tuition fees charged for public university/higher education in 2014?</t>
   </si>
   <si>
     <t>C 3.1.4a: Response</t>
@@ -3893,9 +3890,6 @@
     <t>4.1.3c: Does the required training for teachers include improving the skills necessary for teaching towards the full development of respect for the child’s parents, cultural identity, language, and values, as well as respect for the values of the child’s country and other civilizations?</t>
   </si>
   <si>
-    <t>5.1.2: Are reasonable accommodation measures available for children with disabilities in mainstream schools?</t>
-  </si>
-  <si>
     <t>4.1.2d: Does the national curriculum direct education towards the full development of the child’s responsibilities in a free society, including understanding peace, tolerance, equality, and friendship among all persons and groups?</t>
   </si>
   <si>
@@ -4031,7 +4025,7 @@
     <t>5.2.3a: What percentage of students are not taught in their mother tongue?</t>
   </si>
   <si>
-    <t>3.2.1f: Do national laws forbid discrimination in education on national or social orgin?</t>
+    <t>3.2.1f: Do national laws forbid discrimination in education on national or social origin?</t>
   </si>
   <si>
     <t>3.2.1g: Do national laws forbid discrimination in education on property?</t>
@@ -4620,11 +4614,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="62678399"/>
-        <c:axId val="84295537"/>
+        <c:axId val="82620996"/>
+        <c:axId val="6470355"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="62678399"/>
+        <c:axId val="82620996"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4664,14 +4658,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84295537"/>
+        <c:crossAx val="6470355"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84295537"/>
+        <c:axId val="6470355"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4718,7 +4712,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62678399"/>
+        <c:crossAx val="82620996"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4894,11 +4888,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="40628430"/>
-        <c:axId val="58630995"/>
+        <c:axId val="68488421"/>
+        <c:axId val="65062437"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="40628430"/>
+        <c:axId val="68488421"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4938,14 +4932,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58630995"/>
+        <c:crossAx val="65062437"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58630995"/>
+        <c:axId val="65062437"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4992,7 +4986,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40628430"/>
+        <c:crossAx val="68488421"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5168,11 +5162,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="14087033"/>
-        <c:axId val="49770709"/>
+        <c:axId val="11308388"/>
+        <c:axId val="19037948"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="14087033"/>
+        <c:axId val="11308388"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5212,14 +5206,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49770709"/>
+        <c:crossAx val="19037948"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49770709"/>
+        <c:axId val="19037948"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5266,7 +5260,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14087033"/>
+        <c:crossAx val="11308388"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5430,11 +5424,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="46954228"/>
-        <c:axId val="66304123"/>
+        <c:axId val="62420056"/>
+        <c:axId val="62665089"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="46954228"/>
+        <c:axId val="62420056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5474,14 +5468,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="66304123"/>
+        <c:crossAx val="62665089"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66304123"/>
+        <c:axId val="62665089"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5528,7 +5522,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46954228"/>
+        <c:crossAx val="62420056"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5569,15 +5563,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1361880</xdr:colOff>
+      <xdr:colOff>1388880</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>400680</xdr:colOff>
+      <xdr:colOff>427320</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5585,8 +5579,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20081520" y="4242240"/>
-        <a:ext cx="5846040" cy="2512440"/>
+        <a:off x="20108520" y="4233240"/>
+        <a:ext cx="5845680" cy="2512080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5599,15 +5593,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>679320</xdr:colOff>
+      <xdr:colOff>706320</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>143640</xdr:colOff>
+      <xdr:colOff>170280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5615,8 +5609,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26206200" y="4251600"/>
-        <a:ext cx="6271560" cy="2512440"/>
+        <a:off x="26233200" y="4242600"/>
+        <a:ext cx="6271200" cy="2512080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5629,15 +5623,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1361880</xdr:colOff>
+      <xdr:colOff>1388880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>400680</xdr:colOff>
+      <xdr:colOff>427320</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5645,8 +5639,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20081520" y="6871320"/>
-        <a:ext cx="5846040" cy="2512800"/>
+        <a:off x="20108520" y="6862320"/>
+        <a:ext cx="5845680" cy="2512440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5659,15 +5653,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>688680</xdr:colOff>
+      <xdr:colOff>715680</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>153000</xdr:colOff>
+      <xdr:colOff>179640</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5675,8 +5669,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26215560" y="6871320"/>
-        <a:ext cx="6271560" cy="2512800"/>
+        <a:off x="26242560" y="6862320"/>
+        <a:ext cx="6271200" cy="2512440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5720,9 +5714,9 @@
   <dimension ref="A1:AMF11"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="ZT1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="AMA1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="DH4" activeCellId="0" sqref="DH4"/>
+      <selection pane="topRight" activeCell="AMB11" activeCellId="0" sqref="AMB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13983,7 +13977,7 @@
         <v>78.2</v>
       </c>
       <c r="ALR6" s="3" t="s">
-        <v>1071</v>
+        <v>1059</v>
       </c>
       <c r="ALS6" s="6" t="n">
         <v>0.927</v>
@@ -14027,7 +14021,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1</v>
@@ -14616,7 +14610,7 @@
         <v>0.66</v>
       </c>
       <c r="HF7" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="HG7" s="3" t="n">
         <v>1</v>
@@ -15993,7 +15987,7 @@
         <v>0.66</v>
       </c>
       <c r="ALG7" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="ALH7" s="6" t="n">
         <v>0.83</v>
@@ -16023,7 +16017,7 @@
         <v>96</v>
       </c>
       <c r="ALR7" s="3" t="s">
-        <v>1071</v>
+        <v>1059</v>
       </c>
       <c r="ALS7" s="6" t="n">
         <v>0.98</v>
@@ -16067,7 +16061,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
@@ -16677,7 +16671,7 @@
         <v>0</v>
       </c>
       <c r="HF8" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="HG8" s="3" t="n">
         <v>1</v>
@@ -17616,7 +17610,7 @@
         <v>0</v>
       </c>
       <c r="AAW8" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="AAX8" s="6" t="n">
         <v>0.333</v>
@@ -18135,7 +18129,7 @@
         <v>1</v>
       </c>
       <c r="ALW8" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="ALX8" s="3" t="n">
         <v>0</v>
@@ -18167,7 +18161,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
@@ -18203,13 +18197,13 @@
         <v>0.5</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="P9" s="2" t="n">
         <v>1</v>
@@ -18440,7 +18434,7 @@
         <v>0.25</v>
       </c>
       <c r="CX9" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="CY9" s="2" t="n">
         <v>0</v>
@@ -18648,7 +18642,7 @@
         <v>0.5</v>
       </c>
       <c r="FO9" s="2" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="FP9" s="3" t="n">
         <v>0.962</v>
@@ -19722,7 +19716,7 @@
         <v>0</v>
       </c>
       <c r="AAW9" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="AAX9" s="6" t="n">
         <v>0.666</v>
@@ -20226,7 +20220,7 @@
         <v>1059</v>
       </c>
       <c r="ALR9" s="3" t="s">
-        <v>1071</v>
+        <v>1059</v>
       </c>
       <c r="ALS9" s="6" t="n">
         <v>1</v>
@@ -20292,8 +20286,8 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U20" activeCellId="0" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -20335,92 +20329,92 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>1227</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>1228</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>1229</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>1230</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>1231</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>1232</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>1233</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AD1" s="0" t="s">
         <v>1234</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>1235</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="I2" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>1244</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>1245</v>
-      </c>
       <c r="N2" s="0" t="s">
+        <v>1246</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>1247</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="T2" s="0" t="s">
         <v>1248</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>1249</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
         <v>1250</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="AB2" s="0" t="s">
         <v>1251</v>
       </c>
-      <c r="AB2" s="0" t="s">
-        <v>1252</v>
-      </c>
       <c r="AE2" s="0" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>1267</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>1268</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>1269</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="L3" s="0" t="s">
+        <v>1269</v>
+      </c>
+      <c r="O3" s="0" t="s">
         <v>1270</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>1270</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>1271</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>38</v>
@@ -20432,27 +20426,27 @@
         <v>48</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>33</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>1274</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>1275</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>1276</v>
-      </c>
       <c r="L4" s="0" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>35</v>
@@ -20464,7 +20458,7 @@
         <v>147</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>49</v>
@@ -20473,140 +20467,140 @@
         <v>34</v>
       </c>
       <c r="AF4" s="0" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>1279</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>1280</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="L5" s="0" t="s">
         <v>1281</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="O5" s="0" t="s">
         <v>1282</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>1283</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>61</v>
       </c>
       <c r="U5" s="0" t="s">
+        <v>1283</v>
+      </c>
+      <c r="X5" s="0" t="s">
         <v>1284</v>
       </c>
-      <c r="X5" s="0" t="s">
+      <c r="Z5" s="0" t="s">
         <v>1285</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>1286</v>
       </c>
       <c r="AC5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="AF5" s="0" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>1287</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>1280</v>
+      </c>
+      <c r="O6" s="0" t="s">
         <v>1288</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="R6" s="0" t="s">
         <v>1289</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>1282</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>1281</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>1290</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>1291</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>151</v>
       </c>
       <c r="X6" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AF6" s="0" t="s">
         <v>1292</v>
-      </c>
-      <c r="Z6" s="0" t="s">
-        <v>1293</v>
-      </c>
-      <c r="AF6" s="0" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>1295</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="L7" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>1296</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>1297</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>1293</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>1298</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>1299</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>33</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="AF7" s="0" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="0" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>52</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>34</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="0" t="s">
+        <v>1305</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>1306</v>
+      </c>
+      <c r="O9" s="0" t="s">
         <v>1307</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>1308</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>1309</v>
-      </c>
       <c r="R9" s="0" t="s">
-        <v>1288</v>
+        <v>69</v>
       </c>
       <c r="U9" s="0" t="s">
         <v>35</v>
@@ -20614,13 +20608,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="s">
+        <v>1308</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="O10" s="0" t="s">
         <v>1310</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>1311</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>1312</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>36</v>
@@ -20628,13 +20622,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="0" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20642,7 +20636,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>38</v>
@@ -20650,10 +20644,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="0" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>39</v>
@@ -20661,160 +20655,160 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J14" s="0" t="s">
+        <v>1316</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="U14" s="0" t="s">
         <v>1318</v>
-      </c>
-      <c r="O14" s="0" t="s">
-        <v>1319</v>
-      </c>
-      <c r="U14" s="0" t="s">
-        <v>1320</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="0" t="s">
+        <v>1319</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>1320</v>
+      </c>
+      <c r="U15" s="0" t="s">
         <v>1321</v>
-      </c>
-      <c r="O15" s="0" t="s">
-        <v>1322</v>
-      </c>
-      <c r="U15" s="0" t="s">
-        <v>1323</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="0" t="s">
+        <v>1322</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>1323</v>
+      </c>
+      <c r="U16" s="0" t="s">
         <v>1324</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>1325</v>
-      </c>
-      <c r="U16" s="0" t="s">
-        <v>1326</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="0" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>53</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O18" s="0" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O19" s="0" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O20" s="0" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U21" s="0" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U22" s="0" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U23" s="0" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U24" s="0" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U25" s="0" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U26" s="0" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U27" s="0" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U28" s="0" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U29" s="0" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U30" s="0" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U31" s="0" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U32" s="0" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U33" s="0" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U34" s="0" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U35" s="0" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U36" s="0" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U37" s="0" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U38" s="0" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20824,57 +20818,57 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U40" s="0" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U41" s="0" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U42" s="0" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U43" s="0" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U44" s="0" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U45" s="0" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U46" s="0" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U47" s="0" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U48" s="0" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U49" s="0" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U50" s="0" t="s">
-        <v>1288</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -20895,8 +20889,8 @@
   </sheetPr>
   <dimension ref="A1:CV9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21105,7 +21099,7 @@
       </c>
       <c r="C2" s="0"/>
       <c r="D2" s="2" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
@@ -21202,7 +21196,7 @@
       <c r="CC2" s="0"/>
       <c r="CD2" s="0"/>
       <c r="CE2" s="2" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="CF2" s="0"/>
       <c r="CG2" s="0"/>
@@ -21227,31 +21221,31 @@
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="2" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
       <c r="G3" s="2" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
       <c r="P3" s="2" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="Q3" s="0"/>
       <c r="R3" s="0"/>
@@ -21262,7 +21256,7 @@
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="2" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="Z3" s="0"/>
       <c r="AA3" s="0"/>
@@ -21271,65 +21265,65 @@
       <c r="AD3" s="0"/>
       <c r="AE3" s="0"/>
       <c r="AF3" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="AG3" s="0"/>
       <c r="AH3" s="0"/>
       <c r="AI3" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="AJ3" s="0"/>
       <c r="AK3" s="0"/>
       <c r="AL3" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="AM3" s="0"/>
       <c r="AN3" s="0"/>
       <c r="AO3" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="AP3" s="0"/>
       <c r="AQ3" s="0"/>
       <c r="AR3" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="AS3" s="0"/>
       <c r="AT3" s="0"/>
       <c r="AU3" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="AV3" s="0"/>
       <c r="AW3" s="0"/>
       <c r="AX3" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="AY3" s="0"/>
       <c r="AZ3" s="0"/>
       <c r="BA3" s="0"/>
       <c r="BB3" s="0"/>
       <c r="BC3" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="BD3" s="0"/>
       <c r="BE3" s="0"/>
       <c r="BF3" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="BG3" s="0"/>
       <c r="BH3" s="0"/>
       <c r="BI3" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="BJ3" s="0"/>
       <c r="BK3" s="0"/>
       <c r="BL3" s="0"/>
       <c r="BM3" s="0"/>
       <c r="BN3" s="2" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="BO3" s="0"/>
       <c r="BP3" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="BQ3" s="0"/>
       <c r="BR3" s="0"/>
@@ -21337,11 +21331,11 @@
       <c r="BT3" s="0"/>
       <c r="BU3" s="0"/>
       <c r="BV3" s="2" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="BW3" s="0"/>
       <c r="BX3" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="BY3" s="0"/>
       <c r="BZ3" s="0"/>
@@ -21350,337 +21344,337 @@
       <c r="CC3" s="0"/>
       <c r="CD3" s="0"/>
       <c r="CE3" s="2" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="CF3" s="0"/>
       <c r="CG3" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="CH3" s="0"/>
       <c r="CI3" s="0"/>
       <c r="CJ3" s="2" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="CK3" s="0"/>
       <c r="CL3" s="2" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="CM3" s="0"/>
       <c r="CN3" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="CO3" s="0"/>
       <c r="CP3" s="0"/>
       <c r="CQ3" s="2" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="CR3" s="0"/>
       <c r="CS3" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="CT3" s="0"/>
       <c r="CU3" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="CV3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>1085</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>1115</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>1116</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>1087</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>1117</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>1118</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>1088</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>1119</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>1120</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>1121</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>1122</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>1123</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>1124</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>1125</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>1126</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>1127</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>1128</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>1127</v>
-      </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>1129</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>1130</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>1131</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>1132</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>1133</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AB4" s="2" t="s">
         <v>1134</v>
       </c>
-      <c r="AB4" s="2" t="s">
+      <c r="AC4" s="2" t="s">
         <v>1135</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AD4" s="2" t="s">
         <v>1136</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>1137</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AF4" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AG4" s="3" t="s">
         <v>1138</v>
       </c>
-      <c r="AF4" s="3" t="s">
-        <v>1092</v>
-      </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>1139</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>1140</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>1141</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>1142</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>1143</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>1144</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>1145</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>1146</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>1147</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>1148</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>1149</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>1150</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>1151</v>
       </c>
-      <c r="AT4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="AU4" s="3" t="s">
+      <c r="AV4" s="3" t="s">
         <v>1153</v>
       </c>
-      <c r="AV4" s="3" t="s">
+      <c r="AW4" s="3" t="s">
         <v>1154</v>
       </c>
-      <c r="AW4" s="3" t="s">
+      <c r="AX4" s="3" t="s">
         <v>1155</v>
       </c>
-      <c r="AX4" s="3" t="s">
+      <c r="AY4" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="AY4" s="3" t="s">
+      <c r="AZ4" s="3" t="s">
         <v>1157</v>
       </c>
-      <c r="AZ4" s="3" t="s">
+      <c r="BA4" s="3" t="s">
         <v>1158</v>
       </c>
-      <c r="BA4" s="3" t="s">
+      <c r="BB4" s="3" t="s">
         <v>1159</v>
       </c>
-      <c r="BB4" s="3" t="s">
+      <c r="BC4" s="3" t="s">
         <v>1160</v>
       </c>
-      <c r="BC4" s="3" t="s">
+      <c r="BD4" s="3" t="s">
         <v>1161</v>
       </c>
-      <c r="BD4" s="3" t="s">
+      <c r="BE4" s="3" t="s">
         <v>1162</v>
       </c>
-      <c r="BE4" s="3" t="s">
+      <c r="BF4" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="BG4" s="3" t="s">
         <v>1163</v>
       </c>
-      <c r="BF4" s="3" t="s">
-        <v>1100</v>
-      </c>
-      <c r="BG4" s="3" t="s">
+      <c r="BH4" s="3" t="s">
         <v>1164</v>
       </c>
-      <c r="BH4" s="3" t="s">
+      <c r="BI4" s="3" t="s">
         <v>1165</v>
       </c>
-      <c r="BI4" s="3" t="s">
+      <c r="BJ4" s="3" t="s">
         <v>1166</v>
       </c>
-      <c r="BJ4" s="3" t="s">
+      <c r="BK4" s="3" t="s">
         <v>1167</v>
       </c>
-      <c r="BK4" s="3" t="s">
+      <c r="BL4" s="3" t="s">
         <v>1168</v>
       </c>
-      <c r="BL4" s="3" t="s">
+      <c r="BM4" s="3" t="s">
         <v>1169</v>
       </c>
-      <c r="BM4" s="3" t="s">
+      <c r="BN4" s="2" t="s">
+        <v>1101</v>
+      </c>
+      <c r="BO4" s="2" t="s">
         <v>1170</v>
       </c>
-      <c r="BN4" s="2" t="s">
-        <v>1102</v>
-      </c>
-      <c r="BO4" s="2" t="s">
+      <c r="BP4" s="3" t="s">
         <v>1171</v>
       </c>
-      <c r="BP4" s="3" t="s">
+      <c r="BQ4" s="3" t="s">
         <v>1172</v>
       </c>
-      <c r="BQ4" s="3" t="s">
+      <c r="BR4" s="3" t="s">
         <v>1173</v>
       </c>
-      <c r="BR4" s="3" t="s">
+      <c r="BS4" s="3" t="s">
         <v>1174</v>
       </c>
-      <c r="BS4" s="3" t="s">
+      <c r="BT4" s="3" t="s">
         <v>1175</v>
       </c>
-      <c r="BT4" s="3" t="s">
+      <c r="BU4" s="3" t="s">
         <v>1176</v>
       </c>
-      <c r="BU4" s="3" t="s">
+      <c r="BV4" s="2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="BW4" s="2" t="s">
         <v>1177</v>
       </c>
-      <c r="BV4" s="2" t="s">
-        <v>1104</v>
-      </c>
-      <c r="BW4" s="2" t="s">
+      <c r="BX4" s="3" t="s">
         <v>1178</v>
       </c>
-      <c r="BX4" s="3" t="s">
+      <c r="BY4" s="3" t="s">
         <v>1179</v>
       </c>
-      <c r="BY4" s="3" t="s">
+      <c r="BZ4" s="3" t="s">
         <v>1180</v>
       </c>
-      <c r="BZ4" s="3" t="s">
+      <c r="CA4" s="3" t="s">
         <v>1181</v>
       </c>
-      <c r="CA4" s="3" t="s">
+      <c r="CB4" s="3" t="s">
         <v>1182</v>
       </c>
-      <c r="CB4" s="3" t="s">
+      <c r="CC4" s="3" t="s">
         <v>1183</v>
       </c>
-      <c r="CC4" s="3" t="s">
+      <c r="CD4" s="3" t="s">
         <v>1184</v>
       </c>
-      <c r="CD4" s="3" t="s">
+      <c r="CE4" s="2" t="s">
+        <v>1105</v>
+      </c>
+      <c r="CF4" s="2" t="s">
         <v>1185</v>
       </c>
-      <c r="CE4" s="2" t="s">
+      <c r="CG4" s="3" t="s">
         <v>1106</v>
       </c>
-      <c r="CF4" s="2" t="s">
+      <c r="CH4" s="3" t="s">
         <v>1186</v>
       </c>
-      <c r="CG4" s="3" t="s">
+      <c r="CI4" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="CJ4" s="2" t="s">
         <v>1107</v>
       </c>
-      <c r="CH4" s="3" t="s">
-        <v>1187</v>
-      </c>
-      <c r="CI4" s="3" t="s">
+      <c r="CK4" s="2" t="s">
         <v>1188</v>
       </c>
-      <c r="CJ4" s="2" t="s">
+      <c r="CL4" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="CK4" s="2" t="s">
+      <c r="CM4" s="2" t="s">
         <v>1189</v>
       </c>
-      <c r="CL4" s="2" t="s">
+      <c r="CN4" s="3" t="s">
         <v>1109</v>
       </c>
-      <c r="CM4" s="2" t="s">
+      <c r="CO4" s="3" t="s">
         <v>1190</v>
       </c>
-      <c r="CN4" s="3" t="s">
+      <c r="CP4" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="CQ4" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="CO4" s="3" t="s">
-        <v>1191</v>
-      </c>
-      <c r="CP4" s="3" t="s">
+      <c r="CR4" s="2" t="s">
         <v>1192</v>
       </c>
-      <c r="CQ4" s="2" t="s">
+      <c r="CS4" s="3" t="s">
         <v>1111</v>
       </c>
-      <c r="CR4" s="2" t="s">
+      <c r="CT4" s="3" t="s">
         <v>1193</v>
       </c>
-      <c r="CS4" s="3" t="s">
+      <c r="CU4" s="3" t="s">
         <v>1112</v>
       </c>
-      <c r="CT4" s="3" t="s">
+      <c r="CV4" s="3" t="s">
         <v>1194</v>
-      </c>
-      <c r="CU4" s="3" t="s">
-        <v>1113</v>
-      </c>
-      <c r="CV4" s="3" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21835,10 +21829,10 @@
         <v>1052</v>
       </c>
       <c r="BK5" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="BL5" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="BM5" s="3" t="n">
         <v>2012</v>
@@ -22179,7 +22173,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1</v>
@@ -22355,10 +22349,10 @@
         <v>1052</v>
       </c>
       <c r="BK7" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="BL7" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="BM7" s="3" t="n">
         <v>2013</v>
@@ -22452,7 +22446,7 @@
         <v>0.66</v>
       </c>
       <c r="CT7" s="3" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="CV7" s="3" t="s">
         <v>1059</v>
@@ -22460,7 +22454,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
@@ -22632,10 +22626,10 @@
         <v>1052</v>
       </c>
       <c r="BK8" s="3" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="BL8" s="3" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="BM8" s="3" t="n">
         <v>2015</v>
@@ -22733,7 +22727,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
@@ -22883,10 +22877,10 @@
         <v>1052</v>
       </c>
       <c r="BK9" s="3" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="BL9" s="3" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="BM9" s="3" t="n">
         <v>2015</v>
@@ -23016,7 +23010,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B2" s="11" t="n">
         <f aca="false">AVERAGE(B3,B9,B14,B18,B22)</f>
@@ -23025,7 +23019,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B3" s="13" t="n">
         <f aca="false">AVERAGE(B4:B8)</f>
@@ -23034,7 +23028,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B4" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!BP5*100)</f>
@@ -23043,7 +23037,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B5" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CI5*100)</f>
@@ -23052,7 +23046,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B6" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CP5*100)</f>
@@ -23061,7 +23055,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B7" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EF5*100)</f>
@@ -23070,7 +23064,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B8" s="15" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!AME5,'Core Questionnaire'!ALT5,'Core Questionnaire'!ALI5,'Core Questionnaire'!ALB5,'Core Questionnaire'!AAY5,'Core Questionnaire'!AAP5,'Core Questionnaire'!ZA5,'Core Questionnaire'!HJ5,'Core Questionnaire'!FT5,'Core Questionnaire'!FL5,'Core Questionnaire'!FF5,'Core Questionnaire'!EW5,'Core Questionnaire'!EN5,'Core Questionnaire'!EG5,'Core Questionnaire'!CQ5,'Core Questionnaire'!CJ5,'Core Questionnaire'!BQ5)*100</f>
@@ -23083,7 +23077,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">AVERAGE(B10:B13)</f>
@@ -23092,7 +23086,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B10" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EM5*100)</f>
@@ -23101,7 +23095,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B11" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EV5*100)</f>
@@ -23110,7 +23104,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B12" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FE5*100)</f>
@@ -23119,7 +23113,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B13" s="14" t="n">
         <f aca="false">IF('Core Questionnaire'!FK5&gt;=1,"1",'Core Questionnaire'!FK5)*100</f>
@@ -23132,7 +23126,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B14" s="13" t="n">
         <f aca="false">AVERAGE(B15:B17)</f>
@@ -23141,7 +23135,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B15" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FS5*100)</f>
@@ -23150,7 +23144,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B16" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!HI5*100)</f>
@@ -23159,7 +23153,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B17" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!YZ5*100)</f>
@@ -23172,7 +23166,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" s="13" t="n">
         <f aca="false">AVERAGE(B19:B21)</f>
@@ -23181,7 +23175,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B19" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAO5*100)</f>
@@ -23190,7 +23184,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B20" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAX5*100)</f>
@@ -23199,7 +23193,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALA5*100)</f>
@@ -23212,7 +23206,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" s="13" t="n">
         <f aca="false">AVERAGE(B23:B25)</f>
@@ -23221,7 +23215,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALH5*100)</f>
@@ -23230,7 +23224,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B24" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALS5*100)</f>
@@ -23239,7 +23233,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B25" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AMD5*100)</f>
@@ -23290,7 +23284,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B2" s="11" t="n">
         <f aca="false">AVERAGE(B3,B9,B14,B18,B22)</f>
@@ -23299,7 +23293,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B3" s="13" t="n">
         <f aca="false">AVERAGE(B4:B8)</f>
@@ -23308,7 +23302,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B4" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!BP6*100)</f>
@@ -23317,7 +23311,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B5" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CI6*100)</f>
@@ -23326,7 +23320,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B6" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CP6*100)</f>
@@ -23335,7 +23329,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B7" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EF6*100)</f>
@@ -23344,7 +23338,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B8" s="16" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!AME6,'Core Questionnaire'!ALT6,'Core Questionnaire'!ALI6,'Core Questionnaire'!ALB6,'Core Questionnaire'!AAY6,'Core Questionnaire'!AAP6,'Core Questionnaire'!ZA6,'Core Questionnaire'!HJ6,'Core Questionnaire'!FT6,'Core Questionnaire'!FL6,'Core Questionnaire'!FF6,'Core Questionnaire'!EW6,'Core Questionnaire'!EN6,'Core Questionnaire'!EG6,'Core Questionnaire'!CQ6,'Core Questionnaire'!CJ6,'Core Questionnaire'!BQ6)*100</f>
@@ -23357,7 +23351,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">AVERAGE(B10:B13)</f>
@@ -23366,7 +23360,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B10" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EM6*100)</f>
@@ -23375,7 +23369,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B11" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EV6*100)</f>
@@ -23384,7 +23378,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B12" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FE6*100)</f>
@@ -23393,7 +23387,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B13" s="14" t="n">
         <f aca="false">IF('Core Questionnaire'!FK6&gt;=1,"1",'Core Questionnaire'!FK6)*100</f>
@@ -23406,7 +23400,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B14" s="13" t="n">
         <f aca="false">AVERAGE(B15:B17)</f>
@@ -23415,7 +23409,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B15" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FS6*100)</f>
@@ -23424,7 +23418,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B16" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!HI6*100)</f>
@@ -23433,7 +23427,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B17" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!YZ6*100)</f>
@@ -23446,7 +23440,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" s="13" t="n">
         <f aca="false">AVERAGE(B19:B21)</f>
@@ -23455,7 +23449,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B19" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAO6*100)</f>
@@ -23464,7 +23458,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B20" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAX6*100)</f>
@@ -23473,7 +23467,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" s="14" t="n">
         <v>80.6</v>
@@ -23485,7 +23479,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" s="13" t="n">
         <f aca="false">AVERAGE(B23:B25)</f>
@@ -23494,7 +23488,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALH6*100)</f>
@@ -23503,7 +23497,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B24" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALS6*100)</f>
@@ -23512,7 +23506,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B25" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AMD6*100)</f>
@@ -23558,12 +23552,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B2" s="11" t="n">
         <f aca="false">AVERAGE(B3,B9,B14,B18,B22)</f>
@@ -23572,7 +23566,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B3" s="13" t="n">
         <f aca="false">AVERAGE(B4:B8)</f>
@@ -23581,7 +23575,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B4" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!BP7*100)</f>
@@ -23590,7 +23584,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B5" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CI7*100)</f>
@@ -23599,7 +23593,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B6" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CP7*100)</f>
@@ -23608,7 +23602,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B7" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EF7*100)</f>
@@ -23617,7 +23611,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B8" s="14" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!AME7,'Core Questionnaire'!ALT7,'Core Questionnaire'!ALI7,'Core Questionnaire'!ALB7,'Core Questionnaire'!AAY7,'Core Questionnaire'!AAP7,'Core Questionnaire'!ZA7,'Core Questionnaire'!HJ7,'Core Questionnaire'!FT7,'Core Questionnaire'!FL7,'Core Questionnaire'!FF7,'Core Questionnaire'!EW7,'Core Questionnaire'!EN7,'Core Questionnaire'!EG7,'Core Questionnaire'!CQ7,'Core Questionnaire'!CJ7,'Core Questionnaire'!BQ7)*100</f>
@@ -23626,7 +23620,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">AVERAGE(B10:B13)</f>
@@ -23635,7 +23629,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B10" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EM7*100)</f>
@@ -23644,7 +23638,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B11" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EV7*100)</f>
@@ -23653,7 +23647,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B12" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FE7*100)</f>
@@ -23662,7 +23656,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B13" s="14" t="n">
         <f aca="false">IF('Core Questionnaire'!FK7&gt;=1,"1",'Core Questionnaire'!FK7)*100</f>
@@ -23671,7 +23665,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B14" s="13" t="n">
         <f aca="false">AVERAGE(B15:B17)</f>
@@ -23680,7 +23674,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B15" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FS7*100)</f>
@@ -23689,7 +23683,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B16" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!HI7*100)</f>
@@ -23698,7 +23692,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B17" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!YZ7*100)</f>
@@ -23707,7 +23701,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" s="13" t="n">
         <f aca="false">AVERAGE(B19:B21)</f>
@@ -23716,7 +23710,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B19" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAO7*100)</f>
@@ -23725,7 +23719,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B20" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAX7*100)</f>
@@ -23734,7 +23728,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALA7*100)</f>
@@ -23743,7 +23737,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" s="13" t="n">
         <f aca="false">AVERAGE(B23:B25)</f>
@@ -23752,7 +23746,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALH7*100)</f>
@@ -23761,7 +23755,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B24" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALS7*100)</f>
@@ -23770,7 +23764,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B25" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AMD7*100)</f>
@@ -23812,12 +23806,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B2" s="11" t="n">
         <f aca="false">AVERAGE(B3,B9,B14,B18,B22)</f>
@@ -23826,7 +23820,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B3" s="13" t="n">
         <f aca="false">AVERAGE(B4:B8)</f>
@@ -23835,7 +23829,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B4" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!BP8*100)</f>
@@ -23844,7 +23838,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B5" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CI8*100)</f>
@@ -23853,7 +23847,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B6" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CP8*100)</f>
@@ -23862,7 +23856,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B7" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EF8*100)</f>
@@ -23871,7 +23865,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B8" s="14" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!AME8,'Core Questionnaire'!ALT8,'Core Questionnaire'!ALI8,'Core Questionnaire'!ALB8,'Core Questionnaire'!AAY8,'Core Questionnaire'!AAP8,'Core Questionnaire'!ZA8,'Core Questionnaire'!HJ8,'Core Questionnaire'!FT8,'Core Questionnaire'!FL8,'Core Questionnaire'!FF8,'Core Questionnaire'!EW8,'Core Questionnaire'!EN8,'Core Questionnaire'!EG8,'Core Questionnaire'!CQ8,'Core Questionnaire'!CJ8,'Core Questionnaire'!BQ8)*100</f>
@@ -23880,7 +23874,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">AVERAGE(B10:B13)</f>
@@ -23889,7 +23883,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B10" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EM8*100)</f>
@@ -23898,7 +23892,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B11" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EV8*100)</f>
@@ -23907,7 +23901,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B12" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FE8*100)</f>
@@ -23916,7 +23910,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B13" s="14" t="n">
         <f aca="false">IF('Core Questionnaire'!FK8&gt;=1,"1", 'Core Questionnaire'!FK8)*100</f>
@@ -23925,7 +23919,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B14" s="13" t="n">
         <f aca="false">AVERAGE(B15:B17)</f>
@@ -23934,7 +23928,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B15" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FS8*100)</f>
@@ -23943,7 +23937,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B16" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!HI8*100)</f>
@@ -23952,7 +23946,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B17" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!YZ8*100)</f>
@@ -23961,7 +23955,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" s="13" t="n">
         <f aca="false">AVERAGE(B19:B21)</f>
@@ -23970,7 +23964,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B19" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAO8*100)</f>
@@ -23979,7 +23973,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B20" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAX8*100)</f>
@@ -23988,7 +23982,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALA8*100)</f>
@@ -23997,7 +23991,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" s="13" t="n">
         <f aca="false">AVERAGE(B23:B25)</f>
@@ -24006,7 +24000,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALH8*100)</f>
@@ -24015,7 +24009,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B24" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALS8*100)</f>
@@ -24024,7 +24018,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B25" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AMD8*100)</f>
@@ -24066,12 +24060,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="9" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B2" s="11" t="n">
         <f aca="false">AVERAGE(B3,B9,B14,B18,B22)</f>
@@ -24080,7 +24074,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B3" s="13" t="n">
         <f aca="false">AVERAGE(B4:B8)</f>
@@ -24089,7 +24083,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B4" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!BP9*100)</f>
@@ -24098,7 +24092,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B5" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CI9*100)</f>
@@ -24107,7 +24101,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B6" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!CP9*100)</f>
@@ -24116,7 +24110,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B7" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EF9*100)</f>
@@ -24125,7 +24119,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B8" s="14" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!AME9,'Core Questionnaire'!ALT9,'Core Questionnaire'!ALI9,'Core Questionnaire'!ALB9,'Core Questionnaire'!AAY9,'Core Questionnaire'!AAP9,'Core Questionnaire'!ZA9,'Core Questionnaire'!HJ9,'Core Questionnaire'!FT9,'Core Questionnaire'!FL9,'Core Questionnaire'!FF9,'Core Questionnaire'!EW9,'Core Questionnaire'!EN9,'Core Questionnaire'!EG9,'Core Questionnaire'!CQ9,'Core Questionnaire'!CJ9,'Core Questionnaire'!BQ9)*100</f>
@@ -24134,7 +24128,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">AVERAGE(B10:B13)</f>
@@ -24143,7 +24137,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B10" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EM9*100)</f>
@@ -24152,7 +24146,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B11" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!EV9*100)</f>
@@ -24161,7 +24155,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B12" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FE9*100)</f>
@@ -24170,7 +24164,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B13" s="14" t="n">
         <f aca="false">IF('Core Questionnaire'!FK9&gt;=1,"1", 'Core Questionnaire'!FK9)*100</f>
@@ -24179,7 +24173,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B14" s="13" t="n">
         <f aca="false">AVERAGE(B15:B17)</f>
@@ -24188,7 +24182,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B15" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!FS9*100)</f>
@@ -24197,7 +24191,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B16" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!HI9*100)</f>
@@ -24206,7 +24200,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B17" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!YZ9*100)</f>
@@ -24215,7 +24209,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B18" s="13" t="n">
         <f aca="false">AVERAGE(B19:B21)</f>
@@ -24224,7 +24218,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B19" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAO9*100)</f>
@@ -24233,7 +24227,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B20" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AAX9*100)</f>
@@ -24242,7 +24236,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B21" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALA9*100)</f>
@@ -24251,7 +24245,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B22" s="13" t="n">
         <f aca="false">AVERAGE(B23:B25)</f>
@@ -24260,7 +24254,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B23" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALH9*100)</f>
@@ -24269,7 +24263,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B24" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!ALS9*100)</f>
@@ -24278,7 +24272,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B25" s="14" t="n">
         <f aca="false">PRODUCT('Core Questionnaire'!AMD9*100)</f>
@@ -24326,7 +24320,7 @@
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17"/>
       <c r="B1" s="17" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="19"/>
@@ -24337,18 +24331,18 @@
         <v>1069</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B2" s="22" t="n">
         <f aca="false">J2</f>
@@ -24357,7 +24351,7 @@
       <c r="D2" s="23"/>
       <c r="E2" s="24"/>
       <c r="G2" s="10" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="H2" s="11" t="n">
         <f aca="false">'Chile Summary'!B2</f>
@@ -24391,7 +24385,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="24"/>
       <c r="G3" s="12" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="H3" s="13" t="n">
         <f aca="false">'Chile Summary'!B3</f>
@@ -24425,7 +24419,7 @@
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
       <c r="G4" s="0" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="H4" s="14" t="n">
         <f aca="false">'Chile Summary'!B4</f>
@@ -24450,7 +24444,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B5" s="22" t="n">
         <f aca="false">L2</f>
@@ -24459,7 +24453,7 @@
       <c r="D5" s="23"/>
       <c r="E5" s="24"/>
       <c r="G5" s="0" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="H5" s="14" t="n">
         <f aca="false">'Chile Summary'!B5</f>
@@ -24484,7 +24478,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B6" s="22" t="n">
         <f aca="false">K2</f>
@@ -24493,7 +24487,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="24"/>
       <c r="G6" s="0" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="H6" s="14" t="n">
         <f aca="false">'Chile Summary'!B6</f>
@@ -24522,7 +24516,7 @@
       <c r="D7" s="23"/>
       <c r="E7" s="24"/>
       <c r="G7" s="0" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="H7" s="14" t="n">
         <f aca="false">'Chile Summary'!B7</f>
@@ -24548,14 +24542,14 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="26"/>
       <c r="B8" s="26" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H8" s="14" t="n">
         <f aca="false">'Chile Summary'!B8</f>
@@ -24594,7 +24588,7 @@
         <v>75.625</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="H9" s="13" t="n">
         <f aca="false">'Chile Summary'!B9</f>
@@ -24619,21 +24613,21 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B10" s="27" t="n">
         <f aca="false">J3</f>
         <v>93.1011764705882</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E10" s="27" t="n">
         <f aca="false">L9</f>
         <v>67.35</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="H10" s="14" t="n">
         <f aca="false">'Chile Summary'!B10</f>
@@ -24658,21 +24652,21 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B11" s="27" t="n">
         <f aca="false">K3</f>
         <v>84.1752941176471</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E11" s="27" t="n">
         <f aca="false">J9</f>
         <v>57</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="H11" s="14" t="n">
         <f aca="false">'Chile Summary'!B11</f>
@@ -24713,7 +24707,7 @@
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="0" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">'Chile Summary'!B12</f>
@@ -24738,7 +24732,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B13" s="27" t="n">
         <f aca="false">L3</f>
@@ -24746,7 +24740,7 @@
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="21" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E13" s="27" t="n">
         <f aca="false">K9</f>
@@ -24754,7 +24748,7 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="0" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">'Chile Summary'!B13</f>
@@ -24785,7 +24779,7 @@
       <c r="E14" s="28"/>
       <c r="F14" s="24"/>
       <c r="G14" s="12" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="H14" s="13" t="n">
         <f aca="false">'Chile Summary'!B14</f>
@@ -24811,16 +24805,16 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26"/>
       <c r="B15" s="26" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="F15" s="24"/>
       <c r="G15" s="0" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="H15" s="14" t="n">
         <f aca="false">'Chile Summary'!B15</f>
@@ -24845,7 +24839,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B16" s="27" t="n">
         <f aca="false">J14</f>
@@ -24853,7 +24847,7 @@
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="21" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E16" s="27" t="n">
         <f aca="false">J18</f>
@@ -24861,7 +24855,7 @@
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="0" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="H16" s="14" t="n">
         <f aca="false">'Chile Summary'!B16</f>
@@ -24902,7 +24896,7 @@
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="0" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="H17" s="14" t="n">
         <f aca="false">'Chile Summary'!B17</f>
@@ -24927,7 +24921,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="21" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B18" s="27" t="n">
         <f aca="false">K14</f>
@@ -24943,7 +24937,7 @@
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="12" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="H18" s="13" t="n">
         <f aca="false">'Chile Summary'!B18</f>
@@ -24968,7 +24962,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="21" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B19" s="27" t="n">
         <f aca="false">L14</f>
@@ -24976,7 +24970,7 @@
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="21" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E19" s="27" t="n">
         <f aca="false">L18</f>
@@ -24984,7 +24978,7 @@
       </c>
       <c r="F19" s="24"/>
       <c r="G19" s="0" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H19" s="14" t="n">
         <f aca="false">'Chile Summary'!B19</f>
@@ -25017,7 +25011,7 @@
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="21" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E20" s="27" t="n">
         <f aca="false">K18</f>
@@ -25025,7 +25019,7 @@
       </c>
       <c r="F20" s="24"/>
       <c r="G20" s="0" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="H20" s="14" t="n">
         <f aca="false">'Chile Summary'!B20</f>
@@ -25056,7 +25050,7 @@
       <c r="E21" s="29"/>
       <c r="F21" s="24"/>
       <c r="G21" s="0" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="H21" s="14" t="n">
         <f aca="false">'Chile Summary'!B21</f>
@@ -25082,10 +25076,10 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="26"/>
       <c r="B22" s="26" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="H22" s="13" t="n">
         <f aca="false">'Chile Summary'!B22</f>
@@ -25110,7 +25104,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B23" s="27" t="n">
         <f aca="false">J22</f>
@@ -25119,7 +25113,7 @@
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
       <c r="G23" s="0" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="H23" s="14" t="n">
         <f aca="false">'Chile Summary'!B23</f>
@@ -25153,7 +25147,7 @@
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
       <c r="G24" s="0" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H24" s="14" t="n">
         <f aca="false">'Chile Summary'!B24</f>
@@ -25178,7 +25172,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="21" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B25" s="27" t="n">
         <f aca="false">L22</f>
@@ -25187,7 +25181,7 @@
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
       <c r="G25" s="0" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H25" s="14" t="n">
         <f aca="false">'Chile Summary'!B25</f>
@@ -25229,7 +25223,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="21" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B27" s="27" t="n">
         <f aca="false">K22</f>
@@ -25268,8 +25262,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -25280,7 +25274,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="34" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -25320,50 +25314,50 @@
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="34" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
       <c r="E2" s="34" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="34" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="34" t="s">
+        <v>1229</v>
+      </c>
+      <c r="K2" s="34" t="s">
         <v>1230</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="L2" s="34" t="s">
         <v>1231</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="M2" s="34" t="s">
         <v>1232</v>
-      </c>
-      <c r="M2" s="34" t="s">
-        <v>1233</v>
       </c>
       <c r="N2" s="0"/>
       <c r="O2" s="34" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="P2" s="0"/>
       <c r="Q2" s="0"/>
       <c r="R2" s="34" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="S2" s="0"/>
       <c r="T2" s="34" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="U2" s="0"/>
       <c r="V2" s="34" t="s">
+        <v>1236</v>
+      </c>
+      <c r="W2" s="34" t="s">
         <v>1237</v>
-      </c>
-      <c r="W2" s="34" t="s">
-        <v>1238</v>
       </c>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
@@ -25381,70 +25375,70 @@
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="34" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>1239</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="D3" s="34" t="s">
         <v>1240</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="E3" s="34" t="s">
         <v>1241</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="F3" s="34" t="s">
         <v>1242</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="G3" s="34" t="s">
         <v>1243</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="H3" s="34" t="s">
         <v>1244</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="I3" s="34" t="s">
         <v>1245</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="J3" s="34" t="s">
         <v>1246</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="K3" s="34" t="s">
         <v>1247</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="L3" s="34" t="s">
         <v>1248</v>
       </c>
-      <c r="L3" s="34" t="s">
+      <c r="M3" s="34" t="s">
         <v>1249</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="N3" s="34" t="s">
         <v>1250</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="O3" s="34" t="s">
         <v>1251</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="P3" s="34" t="s">
         <v>1252</v>
       </c>
-      <c r="P3" s="34" t="s">
+      <c r="Q3" s="34" t="s">
         <v>1253</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="R3" s="34" t="s">
         <v>1254</v>
       </c>
-      <c r="R3" s="34" t="s">
+      <c r="S3" s="34" t="s">
         <v>1255</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="T3" s="34" t="s">
         <v>1256</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="U3" s="34" t="s">
         <v>1257</v>
       </c>
-      <c r="U3" s="34" t="s">
+      <c r="V3" s="34" t="s">
         <v>1258</v>
       </c>
-      <c r="V3" s="34" t="s">
+      <c r="W3" s="34" t="s">
         <v>1259</v>
-      </c>
-      <c r="W3" s="34" t="s">
-        <v>1260</v>
       </c>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
@@ -25466,17 +25460,17 @@
         <v>68.4</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E4" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZM$5:$ZU$5,'Core Questionnaire'!$AAI$5:$AAM$5)*100</f>
         <v>100</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="G4" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$DA$5,'Core Questionnaire'!$FX$5,'Core Questionnaire'!$HC$5,'Companion Questionnaire'!$CE$5,'Core Questionnaire'!$HP$5,'Core Questionnaire'!$MP$5,'Core Questionnaire'!$PG$5,'Core Questionnaire'!$UE$5,'Companion Questionnaire'!$CG$5,'Core Questionnaire'!$HE$5,'Core Questionnaire'!$ABE$5,'Core Questionnaire'!$ACK$5,'Core Questionnaire'!$ADQ$5,'Core Questionnaire'!$AIQ$5,'Core Questionnaire'!$AJW$5)*100</f>
@@ -25487,7 +25481,7 @@
         <v>72.0316666666667</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J4" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$CE$5, 'Core Questionnaire'!$CG$5, 'Core Questionnaire'!$CY$5, 'Core Questionnaire'!$DC$5, 'Core Questionnaire'!$DE$5, 'Core Questionnaire'!$DI$5, 'Core Questionnaire'!$DO$5, 'Core Questionnaire'!$DU$5, 'Core Questionnaire'!$FV$5, 'Core Questionnaire'!$FZ$5, 'Core Questionnaire'!$GB$5, 'Core Questionnaire'!$GF$5, 'Core Questionnaire'!$GL$5, 'Core Questionnaire'!$GR$5, 'Core Questionnaire'!$HG$5, 'Core Questionnaire'!$ALK$5, 'Core Questionnaire'!$ALM$5, 'Core Questionnaire'!$ALO$5, 'Core Questionnaire'!$ALQ$5)*100</f>
@@ -25513,29 +25507,29 @@
         <v>66.6666666666667</v>
       </c>
       <c r="P4" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="Q4" s="34" t="s">
         <v>1263</v>
-      </c>
-      <c r="Q4" s="34" t="s">
-        <v>1264</v>
       </c>
       <c r="R4" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZW$5:$AAE$5)*100</f>
         <v>0</v>
       </c>
       <c r="S4" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="T4" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="U4" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="V4" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="W4" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="X4" s="0"/>
       <c r="Y4" s="0"/>
@@ -25557,17 +25551,17 @@
         <v>58.25</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E5" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZM$6:$ZU$6,'Core Questionnaire'!$AAI$6:$AAM$6)*100</f>
         <v>100</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="G5" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$DA$6,'Core Questionnaire'!$FX$6,'Core Questionnaire'!$HC$6,'Companion Questionnaire'!$CE$6,'Core Questionnaire'!$HP$6,'Core Questionnaire'!$MP$6,'Core Questionnaire'!$PG$6,'Core Questionnaire'!$UE$6,'Companion Questionnaire'!$CG$6,'Core Questionnaire'!$HE$6,'Core Questionnaire'!$ABE$6,'Core Questionnaire'!$ACK$6,'Core Questionnaire'!$ADQ$6,'Core Questionnaire'!$AIQ$6,'Core Questionnaire'!$AJW$6)*100</f>
@@ -25578,7 +25572,7 @@
         <v>64</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J5" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$CE$6, 'Core Questionnaire'!$CG$6, 'Core Questionnaire'!$CY$6, 'Core Questionnaire'!$DC$6, 'Core Questionnaire'!$DE$6, 'Core Questionnaire'!$DI$6, 'Core Questionnaire'!$DO$6, 'Core Questionnaire'!$DU$6, 'Core Questionnaire'!$FV$6, 'Core Questionnaire'!$FZ$6, 'Core Questionnaire'!$GB$6, 'Core Questionnaire'!$GF$6, 'Core Questionnaire'!$GL$6, 'Core Questionnaire'!$GR$6, 'Core Questionnaire'!$HG$6, 'Core Questionnaire'!$ALK$6, 'Core Questionnaire'!$ALM$6, 'Core Questionnaire'!$ALO$6, 'Core Questionnaire'!$ALQ$6)*100</f>
@@ -25604,7 +25598,7 @@
         <v>100</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q5" s="34" t="s">
         <v>1059</v>
@@ -25614,19 +25608,19 @@
         <v>100</v>
       </c>
       <c r="S5" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="T5" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="U5" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="V5" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="W5" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="X5" s="0"/>
       <c r="Y5" s="0"/>
@@ -25641,24 +25635,24 @@
     </row>
     <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B6" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$DQ$7,'Core Questionnaire'!$GN$7,'Core Questionnaire'!$ALD$7,'Core Questionnaire'!$ALF$7,'Companion Questionnaire'!$BX$7)*100</f>
         <v>73.272</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E6" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZM$7:$ZU$7,'Core Questionnaire'!$AAI$7:$AAM$7)*100</f>
         <v>100</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="G6" s="36" t="s">
         <v>1059</v>
@@ -25668,7 +25662,7 @@
         <v>91.8333333333333</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J6" s="35" t="n">
         <v>82.12</v>
@@ -25693,29 +25687,29 @@
         <v>100</v>
       </c>
       <c r="P6" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="Q6" s="34" t="s">
         <v>1263</v>
-      </c>
-      <c r="Q6" s="34" t="s">
-        <v>1264</v>
       </c>
       <c r="R6" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZW$7:$AAE$7)*100</f>
         <v>100</v>
       </c>
       <c r="S6" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="T6" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="V6" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="W6" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="X6" s="0"/>
       <c r="Y6" s="0"/>
@@ -25730,24 +25724,24 @@
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B7" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$DQ$8,'Core Questionnaire'!$GN$8,'Core Questionnaire'!$ALD$8,'Core Questionnaire'!$ALF$8,'Companion Questionnaire'!$BX$8)*100</f>
         <v>83.25</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E7" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZM$8:$ZU$8,'Core Questionnaire'!$AAI$8:$AAM$8)*100</f>
         <v>100</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="G7" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$DA$8,'Core Questionnaire'!$FX$8,'Core Questionnaire'!$HC$8,'Companion Questionnaire'!$CE$8,'Core Questionnaire'!$HP$8,'Core Questionnaire'!$MP$8,'Core Questionnaire'!$PG$8,'Core Questionnaire'!$UE$8,'Companion Questionnaire'!$CG$8,'Core Questionnaire'!$HE$8,'Core Questionnaire'!$ABE$8,'Core Questionnaire'!$ACK$8,'Core Questionnaire'!$ADQ$8,'Core Questionnaire'!$AIQ$8,'Core Questionnaire'!$AJW$8)*100</f>
@@ -25758,7 +25752,7 @@
         <v>43.6833333333333</v>
       </c>
       <c r="I7" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J7" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$CE$8, 'Core Questionnaire'!$CG$8, 'Core Questionnaire'!$CY$8, 'Core Questionnaire'!$DC$8, 'Core Questionnaire'!$DE$8, 'Core Questionnaire'!$DI$8, 'Core Questionnaire'!$DO$8, 'Core Questionnaire'!$DU$8, 'Core Questionnaire'!$FV$8, 'Core Questionnaire'!$FZ$8, 'Core Questionnaire'!$GB$8, 'Core Questionnaire'!$GF$8, 'Core Questionnaire'!$GL$8, 'Core Questionnaire'!$GR$8, 'Core Questionnaire'!$HG$8, 'Core Questionnaire'!$ALK$8, 'Core Questionnaire'!$ALM$8, 'Core Questionnaire'!$ALO$8, 'Core Questionnaire'!$ALQ$8)*100</f>
@@ -25784,29 +25778,29 @@
         <v>100</v>
       </c>
       <c r="P7" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="Q7" s="34" t="s">
         <v>1263</v>
-      </c>
-      <c r="Q7" s="34" t="s">
-        <v>1264</v>
       </c>
       <c r="R7" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZW$8:$AAE$8)*100</f>
         <v>100</v>
       </c>
       <c r="S7" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="T7" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="U7" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="V7" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="W7" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="X7" s="0"/>
       <c r="Y7" s="0"/>
@@ -25821,24 +25815,24 @@
     </row>
     <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B8" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$DQ$9,'Core Questionnaire'!$GN$9,'Core Questionnaire'!$ALD$9,'Core Questionnaire'!$ALF$9,'Companion Questionnaire'!$BX$9)*100</f>
         <v>58.25</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E8" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZM$9:$ZU$9,'Core Questionnaire'!$AAI$9:$AAM$9)*100</f>
         <v>100</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="G8" s="35" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$DA$9,'Core Questionnaire'!$FX$9,'Core Questionnaire'!$HC$9,'Companion Questionnaire'!$CE$9,'Core Questionnaire'!$HP$9,'Core Questionnaire'!$MP$9,'Core Questionnaire'!$PG$9,'Core Questionnaire'!$UE$9,'Companion Questionnaire'!$CG$9,'Core Questionnaire'!$HE$9,'Core Questionnaire'!$ABE$9,'Core Questionnaire'!$ACK$9,'Core Questionnaire'!$ADQ$9,'Core Questionnaire'!$AIQ$9,'Core Questionnaire'!$AJW$9)*100</f>
@@ -25849,7 +25843,7 @@
         <v>79.25</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J8" s="35" t="n">
         <v>50</v>
@@ -25874,29 +25868,29 @@
         <v>100</v>
       </c>
       <c r="P8" s="34" t="s">
+        <v>1262</v>
+      </c>
+      <c r="Q8" s="34" t="s">
         <v>1263</v>
-      </c>
-      <c r="Q8" s="34" t="s">
-        <v>1264</v>
       </c>
       <c r="R8" s="34" t="n">
         <f aca="false">AVERAGE('Core Questionnaire'!$ZW$9:$AAE$9)*100</f>
         <v>100</v>
       </c>
       <c r="S8" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="U8" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="V8" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="W8" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="X8" s="0"/>
       <c r="Y8" s="0"/>

</xml_diff>

<commit_message>
Extract strings from data for translation
These include:

This includes:

    * Indicator titles
    * Theme titles
    * Theme mappings indicator titles
    * Questionnaire responses

The output file is always `rtei/translation_strings.py`
</commit_message>
<xml_diff>
--- a/data/rtei_data_2015.xlsx
+++ b/data/rtei_data_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="898" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="898" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Core Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
@@ -4474,7 +4474,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4614,11 +4614,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="82620996"/>
-        <c:axId val="6470355"/>
+        <c:axId val="64911072"/>
+        <c:axId val="73217634"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="82620996"/>
+        <c:axId val="64911072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4658,14 +4658,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="6470355"/>
+        <c:crossAx val="73217634"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6470355"/>
+        <c:axId val="73217634"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4712,7 +4712,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82620996"/>
+        <c:crossAx val="64911072"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4748,7 +4748,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4888,11 +4888,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="68488421"/>
-        <c:axId val="65062437"/>
+        <c:axId val="72905300"/>
+        <c:axId val="35303749"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="68488421"/>
+        <c:axId val="72905300"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4932,14 +4932,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="65062437"/>
+        <c:crossAx val="35303749"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65062437"/>
+        <c:axId val="35303749"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4986,7 +4986,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68488421"/>
+        <c:crossAx val="72905300"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5022,7 +5022,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5162,11 +5162,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="11308388"/>
-        <c:axId val="19037948"/>
+        <c:axId val="45737329"/>
+        <c:axId val="36649255"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="11308388"/>
+        <c:axId val="45737329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5206,14 +5206,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19037948"/>
+        <c:crossAx val="36649255"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19037948"/>
+        <c:axId val="36649255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5260,7 +5260,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="11308388"/>
+        <c:crossAx val="45737329"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5296,7 +5296,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5424,11 +5424,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="62420056"/>
-        <c:axId val="62665089"/>
+        <c:axId val="86788847"/>
+        <c:axId val="25318219"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="62420056"/>
+        <c:axId val="86788847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5468,14 +5468,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62665089"/>
+        <c:crossAx val="25318219"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62665089"/>
+        <c:axId val="25318219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5522,7 +5522,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62420056"/>
+        <c:crossAx val="86788847"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5713,10 +5713,10 @@
   </sheetPr>
   <dimension ref="A1:AMF11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="AMA1" activePane="topRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AMB11" activeCellId="0" sqref="AMB11"/>
+      <selection pane="topRight" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6769,7 +6769,7 @@
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
         <v>77</v>
       </c>
@@ -20286,7 +20286,7 @@
   </sheetPr>
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U20" activeCellId="0" sqref="U20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Match capitalization of themes on data and descriptions
</commit_message>
<xml_diff>
--- a/data/rtei_data_2015.xlsx
+++ b/data/rtei_data_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="898" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="898" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Core Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1364">
   <si>
     <t>Theme</t>
   </si>
@@ -3743,39 +3743,108 @@
     <t>12: Alignment of Education Aims</t>
   </si>
   <si>
+    <t>1A.A: Structure and Support</t>
+  </si>
+  <si>
+    <t>1A.B: Participation and Achievement</t>
+  </si>
+  <si>
+    <t>1A.C: Overall State of Education for Children with Disabilities</t>
+  </si>
+  <si>
+    <t>2A: Content of Curriculum</t>
+  </si>
+  <si>
+    <t>2B: Availability of Textbooks</t>
+  </si>
+  <si>
+    <t>3A: Overall State of Girls' Education</t>
+  </si>
+  <si>
+    <t>3B: Discriminatory Environment</t>
+  </si>
+  <si>
+    <t>3C: Relative State of Girls' Education</t>
+  </si>
+  <si>
+    <t>4A: Discriminatory Environment</t>
+  </si>
+  <si>
+    <t>5A: Strength of Monitoring and Accountability</t>
+  </si>
+  <si>
+    <t>6A: National Normative Framework</t>
+  </si>
+  <si>
+    <t>7A: Legal Restrictions in Opportunity and Indirect costs</t>
+  </si>
+  <si>
+    <t>7B: Opportunity and Indirect Costs in Practice</t>
+  </si>
+  <si>
+    <t>8A: Private education Legal Environment</t>
+  </si>
+  <si>
+    <t>8B.A: Relative Teacher Salary</t>
+  </si>
+  <si>
+    <t>8B.B: Relative Gross Enrollment Patterns</t>
+  </si>
+  <si>
+    <t>9A: Content of Teacher Training</t>
+  </si>
+  <si>
+    <t>9B: Effect of Teacher Training</t>
+  </si>
+  <si>
+    <t>10A: Relative Enrollment and Completion Rates</t>
+  </si>
+  <si>
+    <t>10B: Achievement Across Income Quintiles</t>
+  </si>
+  <si>
+    <t>11A: Relative State of Children in Rural Settings</t>
+  </si>
+  <si>
+    <t>12A: Alignment of Education Aims</t>
+  </si>
+  <si>
+    <t>Data Unavailable</t>
+  </si>
+  <si>
+    <t>See analytic handbook for interpretation</t>
+  </si>
+  <si>
+    <t>See analytic handbook for visual</t>
+  </si>
+  <si>
+    <t>See chart below</t>
+  </si>
+  <si>
+    <t>Level 1: Category</t>
+  </si>
+  <si>
+    <t>Level 2: Transversal Theme</t>
+  </si>
+  <si>
     <t>1A.A: Structure and support</t>
   </si>
   <si>
-    <t>1A.B: Participation and achievement</t>
-  </si>
-  <si>
-    <t>1A.C: Overall state of education for children with disabilities</t>
-  </si>
-  <si>
     <t>2A: Content of curriculum</t>
   </si>
   <si>
-    <t>2B: Availability of textbooks</t>
-  </si>
-  <si>
     <t>3A: Overall state of girls' education</t>
   </si>
   <si>
     <t>3B: Discriminatory environment</t>
   </si>
   <si>
-    <t>3C: Relative state of girls' education</t>
-  </si>
-  <si>
     <t>4A: Discriminatory environment</t>
   </si>
   <si>
     <t>5A: Strength of monitoring and accountability</t>
   </si>
   <si>
-    <t>6A: National Normative Framework</t>
-  </si>
-  <si>
     <t>7A: Legal restrictions in opportunity and indirect costs</t>
   </si>
   <si>
@@ -3785,46 +3854,7 @@
     <t>8A: Private education legal environment</t>
   </si>
   <si>
-    <t>8B.A: Relative teacher salary</t>
-  </si>
-  <si>
-    <t>8B.B: Relative gross enrollment patterns</t>
-  </si>
-  <si>
     <t>9A: Content of teacher training</t>
-  </si>
-  <si>
-    <t>9B: Effect of Teacher Training</t>
-  </si>
-  <si>
-    <t>10A: Relative enrollment and completion rates</t>
-  </si>
-  <si>
-    <t>10B: Achievement across income quintiles</t>
-  </si>
-  <si>
-    <t>11A: Relative state of children in rural settings</t>
-  </si>
-  <si>
-    <t>12A: Alignment of education aims</t>
-  </si>
-  <si>
-    <t>Data Unavailable</t>
-  </si>
-  <si>
-    <t>See analytic handbook for interpretation</t>
-  </si>
-  <si>
-    <t>See analytic handbook for visual</t>
-  </si>
-  <si>
-    <t>See chart below</t>
-  </si>
-  <si>
-    <t>Level 1: Category</t>
-  </si>
-  <si>
-    <t>Level 2: Transversal Theme</t>
   </si>
   <si>
     <t>Level 3: Indicators</t>
@@ -4474,7 +4504,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4614,11 +4644,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64911072"/>
-        <c:axId val="73217634"/>
+        <c:axId val="11779938"/>
+        <c:axId val="91036841"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="64911072"/>
+        <c:axId val="11779938"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4658,14 +4688,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73217634"/>
+        <c:crossAx val="91036841"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73217634"/>
+        <c:axId val="91036841"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4712,7 +4742,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64911072"/>
+        <c:crossAx val="11779938"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4748,7 +4778,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4888,11 +4918,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72905300"/>
-        <c:axId val="35303749"/>
+        <c:axId val="23022365"/>
+        <c:axId val="77285666"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="72905300"/>
+        <c:axId val="23022365"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4932,14 +4962,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="35303749"/>
+        <c:crossAx val="77285666"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35303749"/>
+        <c:axId val="77285666"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4986,7 +5016,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72905300"/>
+        <c:crossAx val="23022365"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5022,7 +5052,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5162,11 +5192,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="45737329"/>
-        <c:axId val="36649255"/>
+        <c:axId val="28195491"/>
+        <c:axId val="87160666"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="45737329"/>
+        <c:axId val="28195491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5206,14 +5236,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="36649255"/>
+        <c:crossAx val="87160666"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36649255"/>
+        <c:axId val="87160666"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5260,7 +5290,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45737329"/>
+        <c:crossAx val="28195491"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5296,7 +5326,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5424,11 +5454,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="86788847"/>
-        <c:axId val="25318219"/>
+        <c:axId val="36629855"/>
+        <c:axId val="10816487"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="86788847"/>
+        <c:axId val="36629855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5468,14 +5498,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="25318219"/>
+        <c:crossAx val="10816487"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25318219"/>
+        <c:axId val="10816487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5522,7 +5552,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="86788847"/>
+        <c:crossAx val="36629855"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5713,7 +5743,7 @@
   </sheetPr>
   <dimension ref="A1:AMF11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B4" activeCellId="0" sqref="B4"/>
@@ -20364,57 +20394,57 @@
         <v>1265</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1238</v>
+        <v>1266</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1241</v>
+        <v>1267</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>1243</v>
+        <v>1268</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>1244</v>
+        <v>1269</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>1246</v>
+        <v>1270</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>1247</v>
+        <v>1271</v>
       </c>
       <c r="T2" s="0" t="s">
         <v>1248</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>1249</v>
+        <v>1272</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>1250</v>
+        <v>1273</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>1251</v>
+        <v>1274</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>1254</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1266</v>
+        <v>1276</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1267</v>
+        <v>1277</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>1268</v>
+        <v>1278</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>1269</v>
+        <v>1279</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>1269</v>
+        <v>1279</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>1270</v>
+        <v>1280</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>38</v>
@@ -20426,27 +20456,27 @@
         <v>48</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>1271</v>
+        <v>1281</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>33</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>1272</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>1273</v>
+        <v>1283</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>1274</v>
+        <v>1284</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>1275</v>
+        <v>1285</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>1275</v>
+        <v>1285</v>
       </c>
       <c r="O4" s="0" t="s">
         <v>35</v>
@@ -20458,7 +20488,7 @@
         <v>147</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>1276</v>
+        <v>1286</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>49</v>
@@ -20467,42 +20497,42 @@
         <v>34</v>
       </c>
       <c r="AF4" s="0" t="s">
-        <v>1277</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>1278</v>
+        <v>1288</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>1279</v>
+        <v>1289</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>1280</v>
+        <v>1290</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>1281</v>
+        <v>1291</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>1282</v>
+        <v>1292</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>61</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>1283</v>
+        <v>1293</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>1284</v>
+        <v>1294</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>1285</v>
+        <v>1295</v>
       </c>
       <c r="AC5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="AF5" s="0" t="s">
-        <v>1286</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20510,94 +20540,94 @@
         <v>69</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>1287</v>
+        <v>1297</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>1281</v>
+        <v>1291</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>1280</v>
+        <v>1290</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>1288</v>
+        <v>1298</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>1289</v>
+        <v>1299</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>151</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>1290</v>
+        <v>1300</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>1291</v>
+        <v>1301</v>
       </c>
       <c r="AF6" s="0" t="s">
-        <v>1292</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>1293</v>
+        <v>1303</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>1294</v>
+        <v>1304</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>1295</v>
+        <v>1305</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>1291</v>
+        <v>1301</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>1296</v>
+        <v>1306</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>1297</v>
+        <v>1307</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>33</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>1298</v>
+        <v>1308</v>
       </c>
       <c r="AF7" s="0" t="s">
-        <v>1299</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="0" t="s">
-        <v>1300</v>
+        <v>1310</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>1301</v>
+        <v>1311</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>52</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>1302</v>
+        <v>1312</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>1303</v>
+        <v>1313</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>34</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>1304</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="0" t="s">
-        <v>1305</v>
+        <v>1315</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>1306</v>
+        <v>1316</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>1307</v>
+        <v>1317</v>
       </c>
       <c r="R9" s="0" t="s">
         <v>69</v>
@@ -20608,13 +20638,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="s">
-        <v>1308</v>
+        <v>1318</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>1309</v>
+        <v>1319</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>1310</v>
+        <v>1320</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>36</v>
@@ -20622,13 +20652,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="0" t="s">
-        <v>1291</v>
+        <v>1301</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>1311</v>
+        <v>1321</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>1312</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20636,7 +20666,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>1313</v>
+        <v>1323</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>38</v>
@@ -20644,10 +20674,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="0" t="s">
-        <v>1314</v>
+        <v>1324</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>1315</v>
+        <v>1325</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>39</v>
@@ -20655,160 +20685,160 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J14" s="0" t="s">
-        <v>1316</v>
+        <v>1326</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>1317</v>
+        <v>1327</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>1318</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J15" s="0" t="s">
-        <v>1319</v>
+        <v>1329</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>1320</v>
+        <v>1330</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>1321</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J16" s="0" t="s">
-        <v>1322</v>
+        <v>1332</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>1323</v>
+        <v>1333</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>1324</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J17" s="0" t="s">
-        <v>1325</v>
+        <v>1335</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>53</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>1326</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O18" s="0" t="s">
-        <v>1327</v>
+        <v>1337</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>1328</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O19" s="0" t="s">
-        <v>1329</v>
+        <v>1339</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>1330</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O20" s="0" t="s">
-        <v>1331</v>
+        <v>1341</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>1332</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U21" s="0" t="s">
-        <v>1333</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U22" s="0" t="s">
-        <v>1334</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U23" s="0" t="s">
-        <v>1335</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U24" s="0" t="s">
-        <v>1336</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U25" s="0" t="s">
-        <v>1337</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U26" s="0" t="s">
-        <v>1338</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U27" s="0" t="s">
-        <v>1339</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U28" s="0" t="s">
-        <v>1340</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U29" s="0" t="s">
-        <v>1341</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U30" s="0" t="s">
-        <v>1342</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U31" s="0" t="s">
-        <v>1280</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U32" s="0" t="s">
-        <v>1343</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U33" s="0" t="s">
-        <v>1344</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U34" s="0" t="s">
-        <v>1345</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U35" s="0" t="s">
-        <v>1346</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U36" s="0" t="s">
-        <v>1347</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U37" s="0" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U38" s="0" t="s">
-        <v>1289</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20818,52 +20848,52 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U40" s="0" t="s">
-        <v>1349</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U41" s="0" t="s">
-        <v>1329</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U42" s="0" t="s">
-        <v>1350</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U43" s="0" t="s">
-        <v>1351</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U44" s="0" t="s">
-        <v>1352</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U45" s="0" t="s">
-        <v>1353</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U46" s="0" t="s">
-        <v>1284</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U47" s="0" t="s">
-        <v>1297</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U48" s="0" t="s">
-        <v>1290</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U49" s="0" t="s">
-        <v>1303</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25262,8 +25292,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>